<commit_message>
siedler session eingetragen 11.09.
</commit_message>
<xml_diff>
--- a/catan_data.xlsx
+++ b/catan_data.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfu\OneDrive\Desktop\Projects\Siedler_Masterdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b1f18c208c1b3c/Desktop/dev/catan_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE32EC2E-9B9E-44F1-926B-8C9A92E83A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="349" documentId="13_ncr:1_{AE32EC2E-9B9E-44F1-926B-8C9A92E83A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BA787F3-97DD-4A5A-B6DD-AE471CB233BE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{83B30B11-FE95-4925-9DB4-CCB67C570BD6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{83B30B11-FE95-4925-9DB4-CCB67C570BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AO$47</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="59">
   <si>
     <t>season</t>
   </si>
@@ -211,6 +214,9 @@
   <si>
     <t>alle Sonder-SP inklusive Metropolen</t>
   </si>
+  <si>
+    <t>Online</t>
+  </si>
 </sst>
 </file>
 
@@ -263,14 +269,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -587,60 +592,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8635BA-0A9D-4832-9FDC-B5CDD32D9D6C}">
-  <dimension ref="A1:AO47"/>
+  <dimension ref="A1:AO56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="I27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H47" sqref="H47"/>
+      <selection pane="bottomRight" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" customWidth="1"/>
-    <col min="12" max="13" width="12.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
-    <col min="16" max="16" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.5546875" customWidth="1"/>
-    <col min="22" max="22" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
+    <row r="1" spans="1:41" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
       <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
@@ -665,7 +662,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -690,10 +687,10 @@
       <c r="H2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>30</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -790,11 +787,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2022</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>44639</v>
       </c>
       <c r="C3">
@@ -921,11 +918,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2022</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>44639</v>
       </c>
       <c r="C4">
@@ -1052,11 +1049,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2022</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>44639</v>
       </c>
       <c r="C5">
@@ -1183,11 +1180,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>44639</v>
       </c>
       <c r="C6">
@@ -1314,11 +1311,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2022</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>44639</v>
       </c>
       <c r="C7">
@@ -1445,11 +1442,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2022</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>44639</v>
       </c>
       <c r="C8">
@@ -1576,11 +1573,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2022</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>44639</v>
       </c>
       <c r="C9">
@@ -1707,11 +1704,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2022</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>44639</v>
       </c>
       <c r="C10">
@@ -1838,11 +1835,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2022</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>44639</v>
       </c>
       <c r="C11">
@@ -1969,11 +1966,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2022</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>44639</v>
       </c>
       <c r="C12">
@@ -2100,11 +2097,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2022</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>44639</v>
       </c>
       <c r="C13">
@@ -2231,11 +2228,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2022</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>44639</v>
       </c>
       <c r="C14">
@@ -2362,11 +2359,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2022</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>44639</v>
       </c>
       <c r="C15">
@@ -2493,11 +2490,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2022</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>44639</v>
       </c>
       <c r="C16">
@@ -2624,11 +2621,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2022</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>44639</v>
       </c>
       <c r="C17">
@@ -2755,11 +2752,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2022</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>44639</v>
       </c>
       <c r="C18">
@@ -2886,11 +2883,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2022</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>44639</v>
       </c>
       <c r="C19">
@@ -3017,11 +3014,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2022</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>44639</v>
       </c>
       <c r="C20">
@@ -3148,11 +3145,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2022</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>44639</v>
       </c>
       <c r="C21">
@@ -3279,11 +3276,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2022</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>44639</v>
       </c>
       <c r="C22">
@@ -3410,11 +3407,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2022</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>44639</v>
       </c>
       <c r="C23">
@@ -3541,11 +3538,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2022</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>44639</v>
       </c>
       <c r="C24">
@@ -3672,11 +3669,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2022</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>44639</v>
       </c>
       <c r="C25">
@@ -3803,11 +3800,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2022</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>44639</v>
       </c>
       <c r="C26">
@@ -3934,11 +3931,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2022</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>44639</v>
       </c>
       <c r="C27">
@@ -4068,11 +4065,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2022</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>44639</v>
       </c>
       <c r="C28">
@@ -4202,11 +4199,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2022</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>44639</v>
       </c>
       <c r="C29">
@@ -4336,11 +4333,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2022</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>44716</v>
       </c>
       <c r="C30">
@@ -4470,11 +4467,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2022</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>44716</v>
       </c>
       <c r="C31">
@@ -4604,11 +4601,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2022</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>44716</v>
       </c>
       <c r="C32">
@@ -4738,11 +4735,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2022</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>44716</v>
       </c>
       <c r="C33">
@@ -4872,11 +4869,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2022</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>44716</v>
       </c>
       <c r="C34">
@@ -5006,11 +5003,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2022</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>44716</v>
       </c>
       <c r="C35">
@@ -5140,11 +5137,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2022</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>44716</v>
       </c>
       <c r="C36">
@@ -5274,11 +5271,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2022</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="5">
         <v>44716</v>
       </c>
       <c r="C37">
@@ -5408,11 +5405,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2022</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>44716</v>
       </c>
       <c r="C38">
@@ -5542,11 +5539,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2022</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="5">
         <v>44716</v>
       </c>
       <c r="C39">
@@ -5676,11 +5673,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2022</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="5">
         <v>44716</v>
       </c>
       <c r="C40">
@@ -5810,11 +5807,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2022</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="5">
         <v>44716</v>
       </c>
       <c r="C41">
@@ -5944,11 +5941,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2022</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="5">
         <v>44716</v>
       </c>
       <c r="C42">
@@ -6078,11 +6075,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2022</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <v>44716</v>
       </c>
       <c r="C43">
@@ -6212,11 +6209,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2022</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="5">
         <v>44716</v>
       </c>
       <c r="C44">
@@ -6346,11 +6343,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2022</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="5">
         <v>44716</v>
       </c>
       <c r="C45">
@@ -6378,7 +6375,7 @@
         <v>31</v>
       </c>
       <c r="K45">
-        <f t="shared" ref="K45:K47" si="260">SUM(N45:U45)</f>
+        <f t="shared" ref="K45:K56" si="260">SUM(N45:U45)</f>
         <v>30</v>
       </c>
       <c r="L45">
@@ -6480,11 +6477,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2022</v>
       </c>
-      <c r="B46" s="6">
+      <c r="B46" s="5">
         <v>44716</v>
       </c>
       <c r="C46">
@@ -6614,11 +6611,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2022</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="5">
         <v>44716</v>
       </c>
       <c r="C47">
@@ -6748,7 +6745,1214 @@
         <v>8</v>
       </c>
     </row>
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2022</v>
+      </c>
+      <c r="B48" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C48">
+        <v>16</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48">
+        <v>9</v>
+      </c>
+      <c r="G48">
+        <v>1</v>
+      </c>
+      <c r="H48">
+        <v>2</v>
+      </c>
+      <c r="I48" t="s">
+        <v>36</v>
+      </c>
+      <c r="J48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="260"/>
+        <v>30</v>
+      </c>
+      <c r="L48">
+        <v>6</v>
+      </c>
+      <c r="M48">
+        <v>5</v>
+      </c>
+      <c r="N48">
+        <v>3</v>
+      </c>
+      <c r="O48">
+        <v>5</v>
+      </c>
+      <c r="P48">
+        <v>5</v>
+      </c>
+      <c r="Q48">
+        <v>4</v>
+      </c>
+      <c r="R48">
+        <v>5</v>
+      </c>
+      <c r="S48">
+        <v>3</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
+      </c>
+      <c r="U48">
+        <v>5</v>
+      </c>
+      <c r="V48">
+        <v>0</v>
+      </c>
+      <c r="W48">
+        <v>0</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <v>0</v>
+      </c>
+      <c r="Z48">
+        <v>0</v>
+      </c>
+      <c r="AA48">
+        <v>0</v>
+      </c>
+      <c r="AB48">
+        <v>0</v>
+      </c>
+      <c r="AC48">
+        <v>0</v>
+      </c>
+      <c r="AD48">
+        <v>0</v>
+      </c>
+      <c r="AE48">
+        <v>1</v>
+      </c>
+      <c r="AF48">
+        <v>0</v>
+      </c>
+      <c r="AG48">
+        <v>1</v>
+      </c>
+      <c r="AH48">
+        <f>SUM(N48:N50)</f>
+        <v>18</v>
+      </c>
+      <c r="AI48">
+        <f>SUM(O48:O50)</f>
+        <v>8</v>
+      </c>
+      <c r="AJ48">
+        <f>SUM(P48:P50)</f>
+        <v>14</v>
+      </c>
+      <c r="AK48">
+        <f t="shared" ref="AK48" si="280">SUM(Q48:Q50)</f>
+        <v>18</v>
+      </c>
+      <c r="AL48">
+        <f t="shared" ref="AL48" si="281">SUM(R48:R50)</f>
+        <v>8</v>
+      </c>
+      <c r="AM48">
+        <f t="shared" ref="AM48" si="282">SUM(S48:S50)</f>
+        <v>18</v>
+      </c>
+      <c r="AN48">
+        <f t="shared" ref="AN48" si="283">SUM(T48:T50)</f>
+        <v>3</v>
+      </c>
+      <c r="AO48">
+        <f t="shared" ref="AO48" si="284">SUM(U48:U50)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2022</v>
+      </c>
+      <c r="B49" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C49">
+        <v>16</v>
+      </c>
+      <c r="D49" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" t="s">
+        <v>13</v>
+      </c>
+      <c r="F49">
+        <v>7</v>
+      </c>
+      <c r="G49">
+        <v>2</v>
+      </c>
+      <c r="H49">
+        <v>3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>32</v>
+      </c>
+      <c r="J49" t="s">
+        <v>32</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="260"/>
+        <v>31</v>
+      </c>
+      <c r="L49">
+        <v>5</v>
+      </c>
+      <c r="M49">
+        <v>4</v>
+      </c>
+      <c r="N49">
+        <v>7</v>
+      </c>
+      <c r="O49">
+        <v>3</v>
+      </c>
+      <c r="P49">
+        <v>7</v>
+      </c>
+      <c r="Q49">
+        <v>5</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>7</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <v>2</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>0</v>
+      </c>
+      <c r="AA49">
+        <v>0</v>
+      </c>
+      <c r="AB49">
+        <v>1</v>
+      </c>
+      <c r="AC49">
+        <v>0</v>
+      </c>
+      <c r="AD49">
+        <v>0</v>
+      </c>
+      <c r="AE49">
+        <v>0</v>
+      </c>
+      <c r="AF49">
+        <v>0</v>
+      </c>
+      <c r="AG49">
+        <v>1</v>
+      </c>
+      <c r="AH49">
+        <f>SUM(N48:N50)</f>
+        <v>18</v>
+      </c>
+      <c r="AI49">
+        <f t="shared" ref="AI49" si="285">SUM(O48:O50)</f>
+        <v>8</v>
+      </c>
+      <c r="AJ49">
+        <f t="shared" ref="AJ49" si="286">SUM(P48:P50)</f>
+        <v>14</v>
+      </c>
+      <c r="AK49">
+        <f t="shared" ref="AK49" si="287">SUM(Q48:Q50)</f>
+        <v>18</v>
+      </c>
+      <c r="AL49">
+        <f t="shared" ref="AL49" si="288">SUM(R48:R50)</f>
+        <v>8</v>
+      </c>
+      <c r="AM49">
+        <f t="shared" ref="AM49" si="289">SUM(S48:S50)</f>
+        <v>18</v>
+      </c>
+      <c r="AN49">
+        <f t="shared" ref="AN49" si="290">SUM(T48:T50)</f>
+        <v>3</v>
+      </c>
+      <c r="AO49">
+        <f t="shared" ref="AO49" si="291">SUM(U48:U50)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2022</v>
+      </c>
+      <c r="B50" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C50">
+        <v>16</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50">
+        <v>13</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>37</v>
+      </c>
+      <c r="J50" t="s">
+        <v>32</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="260"/>
+        <v>33</v>
+      </c>
+      <c r="L50">
+        <v>5</v>
+      </c>
+      <c r="M50">
+        <v>4</v>
+      </c>
+      <c r="N50">
+        <v>8</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>2</v>
+      </c>
+      <c r="Q50">
+        <v>9</v>
+      </c>
+      <c r="R50">
+        <v>3</v>
+      </c>
+      <c r="S50">
+        <v>8</v>
+      </c>
+      <c r="T50">
+        <v>3</v>
+      </c>
+      <c r="U50">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+      <c r="X50">
+        <v>0</v>
+      </c>
+      <c r="Y50">
+        <v>0</v>
+      </c>
+      <c r="Z50">
+        <v>0</v>
+      </c>
+      <c r="AA50">
+        <v>0</v>
+      </c>
+      <c r="AB50">
+        <v>0</v>
+      </c>
+      <c r="AC50">
+        <v>0</v>
+      </c>
+      <c r="AD50">
+        <v>0</v>
+      </c>
+      <c r="AE50">
+        <v>0</v>
+      </c>
+      <c r="AF50">
+        <v>0</v>
+      </c>
+      <c r="AG50">
+        <v>1</v>
+      </c>
+      <c r="AH50">
+        <f>SUM(N48:N50)</f>
+        <v>18</v>
+      </c>
+      <c r="AI50">
+        <f t="shared" ref="AI50" si="292">SUM(O48:O50)</f>
+        <v>8</v>
+      </c>
+      <c r="AJ50">
+        <f t="shared" ref="AJ50" si="293">SUM(P48:P50)</f>
+        <v>14</v>
+      </c>
+      <c r="AK50">
+        <f t="shared" ref="AK50" si="294">SUM(Q48:Q50)</f>
+        <v>18</v>
+      </c>
+      <c r="AL50">
+        <f t="shared" ref="AL50" si="295">SUM(R48:R50)</f>
+        <v>8</v>
+      </c>
+      <c r="AM50">
+        <f t="shared" ref="AM50" si="296">SUM(S48:S50)</f>
+        <v>18</v>
+      </c>
+      <c r="AN50">
+        <f t="shared" ref="AN50" si="297">SUM(T48:T50)</f>
+        <v>3</v>
+      </c>
+      <c r="AO50">
+        <f t="shared" ref="AO50" si="298">SUM(U48:U50)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2022</v>
+      </c>
+      <c r="B51" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+      <c r="D51" t="s">
+        <v>58</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51">
+        <v>12</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <v>2</v>
+      </c>
+      <c r="I51" t="s">
+        <v>36</v>
+      </c>
+      <c r="J51" t="s">
+        <v>33</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="260"/>
+        <v>24</v>
+      </c>
+      <c r="L51">
+        <v>6</v>
+      </c>
+      <c r="M51">
+        <v>5</v>
+      </c>
+      <c r="N51">
+        <v>5</v>
+      </c>
+      <c r="O51">
+        <v>4</v>
+      </c>
+      <c r="P51">
+        <v>4</v>
+      </c>
+      <c r="Q51">
+        <v>3</v>
+      </c>
+      <c r="R51">
+        <v>4</v>
+      </c>
+      <c r="S51">
+        <v>0</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="U51">
+        <v>4</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>0</v>
+      </c>
+      <c r="X51">
+        <v>0</v>
+      </c>
+      <c r="Y51">
+        <v>0</v>
+      </c>
+      <c r="Z51">
+        <v>0</v>
+      </c>
+      <c r="AA51">
+        <v>0</v>
+      </c>
+      <c r="AB51">
+        <v>0</v>
+      </c>
+      <c r="AC51">
+        <v>0</v>
+      </c>
+      <c r="AD51">
+        <v>1</v>
+      </c>
+      <c r="AE51">
+        <v>0</v>
+      </c>
+      <c r="AF51">
+        <v>0</v>
+      </c>
+      <c r="AG51">
+        <v>1</v>
+      </c>
+      <c r="AH51">
+        <f>SUM(N51:N53)</f>
+        <v>19</v>
+      </c>
+      <c r="AI51">
+        <f>SUM(O51:O53)</f>
+        <v>12</v>
+      </c>
+      <c r="AJ51">
+        <f>SUM(P51:P53)</f>
+        <v>9</v>
+      </c>
+      <c r="AK51">
+        <f t="shared" ref="AK51" si="299">SUM(Q51:Q53)</f>
+        <v>18</v>
+      </c>
+      <c r="AL51">
+        <f t="shared" ref="AL51" si="300">SUM(R51:R53)</f>
+        <v>8</v>
+      </c>
+      <c r="AM51">
+        <f t="shared" ref="AM51" si="301">SUM(S51:S53)</f>
+        <v>14</v>
+      </c>
+      <c r="AN51">
+        <f t="shared" ref="AN51" si="302">SUM(T51:T53)</f>
+        <v>0</v>
+      </c>
+      <c r="AO51">
+        <f t="shared" ref="AO51" si="303">SUM(U51:U53)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2022</v>
+      </c>
+      <c r="B52" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C52">
+        <v>16</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52">
+        <v>13</v>
+      </c>
+      <c r="G52">
+        <v>5</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>32</v>
+      </c>
+      <c r="J52" t="s">
+        <v>33</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="260"/>
+        <v>31</v>
+      </c>
+      <c r="L52">
+        <v>6</v>
+      </c>
+      <c r="M52">
+        <v>5</v>
+      </c>
+      <c r="N52">
+        <v>5</v>
+      </c>
+      <c r="O52">
+        <v>3</v>
+      </c>
+      <c r="P52">
+        <v>4</v>
+      </c>
+      <c r="Q52">
+        <v>10</v>
+      </c>
+      <c r="R52">
+        <v>4</v>
+      </c>
+      <c r="S52">
+        <v>5</v>
+      </c>
+      <c r="T52">
+        <v>0</v>
+      </c>
+      <c r="U52">
+        <v>0</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>0</v>
+      </c>
+      <c r="X52">
+        <v>0</v>
+      </c>
+      <c r="Y52">
+        <v>0</v>
+      </c>
+      <c r="Z52">
+        <v>0</v>
+      </c>
+      <c r="AA52">
+        <v>0</v>
+      </c>
+      <c r="AB52">
+        <v>0</v>
+      </c>
+      <c r="AC52">
+        <v>0</v>
+      </c>
+      <c r="AD52">
+        <v>0</v>
+      </c>
+      <c r="AE52">
+        <v>0</v>
+      </c>
+      <c r="AF52">
+        <v>1</v>
+      </c>
+      <c r="AG52">
+        <v>0</v>
+      </c>
+      <c r="AH52">
+        <f>SUM(N51:N53)</f>
+        <v>19</v>
+      </c>
+      <c r="AI52">
+        <f t="shared" ref="AI52" si="304">SUM(O51:O53)</f>
+        <v>12</v>
+      </c>
+      <c r="AJ52">
+        <f t="shared" ref="AJ52" si="305">SUM(P51:P53)</f>
+        <v>9</v>
+      </c>
+      <c r="AK52">
+        <f t="shared" ref="AK52" si="306">SUM(Q51:Q53)</f>
+        <v>18</v>
+      </c>
+      <c r="AL52">
+        <f t="shared" ref="AL52" si="307">SUM(R51:R53)</f>
+        <v>8</v>
+      </c>
+      <c r="AM52">
+        <f t="shared" ref="AM52" si="308">SUM(S51:S53)</f>
+        <v>14</v>
+      </c>
+      <c r="AN52">
+        <f t="shared" ref="AN52" si="309">SUM(T51:T53)</f>
+        <v>0</v>
+      </c>
+      <c r="AO52">
+        <f t="shared" ref="AO52" si="310">SUM(U51:U53)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2022</v>
+      </c>
+      <c r="B53" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C53">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" t="s">
+        <v>13</v>
+      </c>
+      <c r="F53">
+        <v>10</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>3</v>
+      </c>
+      <c r="I53" t="s">
+        <v>37</v>
+      </c>
+      <c r="J53" t="s">
+        <v>33</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="260"/>
+        <v>30</v>
+      </c>
+      <c r="L53">
+        <v>6</v>
+      </c>
+      <c r="M53">
+        <v>4</v>
+      </c>
+      <c r="N53">
+        <v>9</v>
+      </c>
+      <c r="O53">
+        <v>5</v>
+      </c>
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="Q53">
+        <v>5</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>9</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <v>1</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>0</v>
+      </c>
+      <c r="X53">
+        <v>0</v>
+      </c>
+      <c r="Y53">
+        <v>0</v>
+      </c>
+      <c r="Z53">
+        <v>0</v>
+      </c>
+      <c r="AA53">
+        <v>0</v>
+      </c>
+      <c r="AB53">
+        <v>0</v>
+      </c>
+      <c r="AC53">
+        <v>1</v>
+      </c>
+      <c r="AD53">
+        <v>0</v>
+      </c>
+      <c r="AE53">
+        <v>0</v>
+      </c>
+      <c r="AF53">
+        <v>0</v>
+      </c>
+      <c r="AG53">
+        <v>1</v>
+      </c>
+      <c r="AH53">
+        <f>SUM(N51:N53)</f>
+        <v>19</v>
+      </c>
+      <c r="AI53">
+        <f t="shared" ref="AI53" si="311">SUM(O51:O53)</f>
+        <v>12</v>
+      </c>
+      <c r="AJ53">
+        <f t="shared" ref="AJ53" si="312">SUM(P51:P53)</f>
+        <v>9</v>
+      </c>
+      <c r="AK53">
+        <f t="shared" ref="AK53" si="313">SUM(Q51:Q53)</f>
+        <v>18</v>
+      </c>
+      <c r="AL53">
+        <f t="shared" ref="AL53" si="314">SUM(R51:R53)</f>
+        <v>8</v>
+      </c>
+      <c r="AM53">
+        <f t="shared" ref="AM53" si="315">SUM(S51:S53)</f>
+        <v>14</v>
+      </c>
+      <c r="AN53">
+        <f t="shared" ref="AN53" si="316">SUM(T51:T53)</f>
+        <v>0</v>
+      </c>
+      <c r="AO53">
+        <f t="shared" ref="AO53" si="317">SUM(U51:U53)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2022</v>
+      </c>
+      <c r="B54" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C54">
+        <v>16</v>
+      </c>
+      <c r="D54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54">
+        <v>6</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>3</v>
+      </c>
+      <c r="I54" t="s">
+        <v>36</v>
+      </c>
+      <c r="J54" t="s">
+        <v>32</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="260"/>
+        <v>34</v>
+      </c>
+      <c r="L54">
+        <v>5</v>
+      </c>
+      <c r="M54">
+        <v>4</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>4</v>
+      </c>
+      <c r="P54">
+        <v>13</v>
+      </c>
+      <c r="Q54">
+        <v>3</v>
+      </c>
+      <c r="R54">
+        <v>5</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="U54">
+        <v>9</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>0</v>
+      </c>
+      <c r="X54">
+        <v>0</v>
+      </c>
+      <c r="Y54">
+        <v>0</v>
+      </c>
+      <c r="Z54">
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <v>0</v>
+      </c>
+      <c r="AB54">
+        <v>0</v>
+      </c>
+      <c r="AC54">
+        <v>1</v>
+      </c>
+      <c r="AD54">
+        <v>0</v>
+      </c>
+      <c r="AE54">
+        <v>0</v>
+      </c>
+      <c r="AF54">
+        <v>0</v>
+      </c>
+      <c r="AG54">
+        <v>0</v>
+      </c>
+      <c r="AH54">
+        <f>SUM(N54:N56)</f>
+        <v>11</v>
+      </c>
+      <c r="AI54">
+        <f>SUM(O54:O56)</f>
+        <v>24</v>
+      </c>
+      <c r="AJ54">
+        <f>SUM(P54:P56)</f>
+        <v>21</v>
+      </c>
+      <c r="AK54">
+        <f t="shared" ref="AK54" si="318">SUM(Q54:Q56)</f>
+        <v>15</v>
+      </c>
+      <c r="AL54">
+        <f t="shared" ref="AL54" si="319">SUM(R54:R56)</f>
+        <v>7</v>
+      </c>
+      <c r="AM54">
+        <f t="shared" ref="AM54" si="320">SUM(S54:S56)</f>
+        <v>9</v>
+      </c>
+      <c r="AN54">
+        <f t="shared" ref="AN54" si="321">SUM(T54:T56)</f>
+        <v>2</v>
+      </c>
+      <c r="AO54">
+        <f t="shared" ref="AO54" si="322">SUM(U54:U56)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2022</v>
+      </c>
+      <c r="B55" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C55">
+        <v>16</v>
+      </c>
+      <c r="D55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55">
+        <v>8</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55" t="s">
+        <v>32</v>
+      </c>
+      <c r="J55" t="s">
+        <v>32</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="260"/>
+        <v>34</v>
+      </c>
+      <c r="L55">
+        <v>4</v>
+      </c>
+      <c r="M55">
+        <v>4</v>
+      </c>
+      <c r="N55">
+        <v>4</v>
+      </c>
+      <c r="O55">
+        <v>14</v>
+      </c>
+      <c r="P55">
+        <v>5</v>
+      </c>
+      <c r="Q55">
+        <v>7</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>4</v>
+      </c>
+      <c r="T55">
+        <v>0</v>
+      </c>
+      <c r="U55">
+        <v>0</v>
+      </c>
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="W55">
+        <v>0</v>
+      </c>
+      <c r="X55">
+        <v>0</v>
+      </c>
+      <c r="Y55">
+        <v>0</v>
+      </c>
+      <c r="Z55">
+        <v>0</v>
+      </c>
+      <c r="AA55">
+        <v>0</v>
+      </c>
+      <c r="AB55">
+        <v>0</v>
+      </c>
+      <c r="AC55">
+        <v>0</v>
+      </c>
+      <c r="AD55">
+        <v>0</v>
+      </c>
+      <c r="AE55">
+        <v>1</v>
+      </c>
+      <c r="AF55">
+        <v>0</v>
+      </c>
+      <c r="AG55">
+        <v>0</v>
+      </c>
+      <c r="AH55">
+        <f>SUM(N54:N56)</f>
+        <v>11</v>
+      </c>
+      <c r="AI55">
+        <f t="shared" ref="AI55" si="323">SUM(O54:O56)</f>
+        <v>24</v>
+      </c>
+      <c r="AJ55">
+        <f t="shared" ref="AJ55" si="324">SUM(P54:P56)</f>
+        <v>21</v>
+      </c>
+      <c r="AK55">
+        <f t="shared" ref="AK55" si="325">SUM(Q54:Q56)</f>
+        <v>15</v>
+      </c>
+      <c r="AL55">
+        <f t="shared" ref="AL55" si="326">SUM(R54:R56)</f>
+        <v>7</v>
+      </c>
+      <c r="AM55">
+        <f t="shared" ref="AM55" si="327">SUM(S54:S56)</f>
+        <v>9</v>
+      </c>
+      <c r="AN55">
+        <f t="shared" ref="AN55" si="328">SUM(T54:T56)</f>
+        <v>2</v>
+      </c>
+      <c r="AO55">
+        <f t="shared" ref="AO55" si="329">SUM(U54:U56)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>2022</v>
+      </c>
+      <c r="B56" s="5">
+        <v>44815</v>
+      </c>
+      <c r="C56">
+        <v>16</v>
+      </c>
+      <c r="D56" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56">
+        <v>13</v>
+      </c>
+      <c r="G56">
+        <v>4</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>37</v>
+      </c>
+      <c r="J56" t="s">
+        <v>32</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="260"/>
+        <v>30</v>
+      </c>
+      <c r="L56">
+        <v>5</v>
+      </c>
+      <c r="M56">
+        <v>5</v>
+      </c>
+      <c r="N56">
+        <v>7</v>
+      </c>
+      <c r="O56">
+        <v>6</v>
+      </c>
+      <c r="P56">
+        <v>3</v>
+      </c>
+      <c r="Q56">
+        <v>5</v>
+      </c>
+      <c r="R56">
+        <v>2</v>
+      </c>
+      <c r="S56">
+        <v>5</v>
+      </c>
+      <c r="T56">
+        <v>2</v>
+      </c>
+      <c r="U56">
+        <v>0</v>
+      </c>
+      <c r="V56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <v>0</v>
+      </c>
+      <c r="X56">
+        <v>0</v>
+      </c>
+      <c r="Y56">
+        <v>0</v>
+      </c>
+      <c r="Z56">
+        <v>0</v>
+      </c>
+      <c r="AA56">
+        <v>0</v>
+      </c>
+      <c r="AB56">
+        <v>0</v>
+      </c>
+      <c r="AC56">
+        <v>0</v>
+      </c>
+      <c r="AD56">
+        <v>0</v>
+      </c>
+      <c r="AE56">
+        <v>0</v>
+      </c>
+      <c r="AF56">
+        <v>0</v>
+      </c>
+      <c r="AG56">
+        <v>0</v>
+      </c>
+      <c r="AH56">
+        <f>SUM(N54:N56)</f>
+        <v>11</v>
+      </c>
+      <c r="AI56">
+        <f t="shared" ref="AI56" si="330">SUM(O54:O56)</f>
+        <v>24</v>
+      </c>
+      <c r="AJ56">
+        <f t="shared" ref="AJ56" si="331">SUM(P54:P56)</f>
+        <v>21</v>
+      </c>
+      <c r="AK56">
+        <f t="shared" ref="AK56" si="332">SUM(Q54:Q56)</f>
+        <v>15</v>
+      </c>
+      <c r="AL56">
+        <f t="shared" ref="AL56" si="333">SUM(R54:R56)</f>
+        <v>7</v>
+      </c>
+      <c r="AM56">
+        <f t="shared" ref="AM56" si="334">SUM(S54:S56)</f>
+        <v>9</v>
+      </c>
+      <c r="AN56">
+        <f t="shared" ref="AN56" si="335">SUM(T54:T56)</f>
+        <v>2</v>
+      </c>
+      <c r="AO56">
+        <f t="shared" ref="AO56" si="336">SUM(U54:U56)</f>
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A2:AO47" xr:uid="{FF8635BA-0A9D-4832-9FDC-B5CDD32D9D6C}"/>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X3:AA8 V3:W41 X9:Y41 V44:Y1048576" xr:uid="{0D054DE4-3D8E-4484-9FF1-661236EA2207}">
       <formula1>0</formula1>
@@ -6792,9 +7996,9 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -6805,7 +8009,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6816,7 +8020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
neue daten - saisonabschluss
</commit_message>
<xml_diff>
--- a/catan_data.xlsx
+++ b/catan_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfu\OneDrive\Desktop\Projects\dev\catan_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB9B884-6B2C-4700-B874-AEAFF0384B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531966C6-6828-4727-A14D-C6D24CC005A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{83B30B11-FE95-4925-9DB4-CCB67C570BD6}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="59">
   <si>
     <t>season</t>
   </si>
@@ -592,13 +592,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8635BA-0A9D-4832-9FDC-B5CDD32D9D6C}">
-  <dimension ref="A1:AO77"/>
+  <dimension ref="A1:AO92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="M76" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J78" sqref="J78"/>
+      <selection pane="bottomRight" activeCell="H84" sqref="H84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6375,7 +6375,7 @@
         <v>31</v>
       </c>
       <c r="K45">
-        <f t="shared" ref="K45:K77" si="260">SUM(N45:U45)</f>
+        <f t="shared" ref="K45:K92" si="260">SUM(N45:U45)</f>
         <v>30</v>
       </c>
       <c r="L45">
@@ -10763,6 +10763,1818 @@
       <c r="AO77">
         <f t="shared" ref="AO77" si="465">SUM(U75:U77)</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>2022</v>
+      </c>
+      <c r="B78" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C78">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>46</v>
+      </c>
+      <c r="E78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78">
+        <v>11</v>
+      </c>
+      <c r="G78">
+        <v>4</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78" t="s">
+        <v>36</v>
+      </c>
+      <c r="J78" t="s">
+        <v>31</v>
+      </c>
+      <c r="K78">
+        <f t="shared" si="260"/>
+        <v>28</v>
+      </c>
+      <c r="L78">
+        <v>5</v>
+      </c>
+      <c r="M78">
+        <v>5</v>
+      </c>
+      <c r="N78">
+        <v>3</v>
+      </c>
+      <c r="O78">
+        <v>6</v>
+      </c>
+      <c r="P78">
+        <v>5</v>
+      </c>
+      <c r="Q78">
+        <v>3</v>
+      </c>
+      <c r="R78">
+        <v>6</v>
+      </c>
+      <c r="S78">
+        <v>3</v>
+      </c>
+      <c r="T78">
+        <v>2</v>
+      </c>
+      <c r="U78">
+        <v>0</v>
+      </c>
+      <c r="V78">
+        <v>0</v>
+      </c>
+      <c r="W78">
+        <v>0</v>
+      </c>
+      <c r="X78">
+        <v>0</v>
+      </c>
+      <c r="Y78">
+        <v>0</v>
+      </c>
+      <c r="Z78">
+        <v>0</v>
+      </c>
+      <c r="AA78">
+        <v>0</v>
+      </c>
+      <c r="AB78">
+        <v>0</v>
+      </c>
+      <c r="AC78">
+        <v>0</v>
+      </c>
+      <c r="AD78">
+        <v>0</v>
+      </c>
+      <c r="AE78">
+        <v>1</v>
+      </c>
+      <c r="AF78">
+        <v>0</v>
+      </c>
+      <c r="AG78">
+        <v>0</v>
+      </c>
+      <c r="AH78">
+        <f>SUM(N78:N80)</f>
+        <v>9</v>
+      </c>
+      <c r="AI78">
+        <f t="shared" ref="AI78" si="466">SUM(O78:O80)</f>
+        <v>21</v>
+      </c>
+      <c r="AJ78">
+        <f t="shared" ref="AJ78" si="467">SUM(P78:P80)</f>
+        <v>12</v>
+      </c>
+      <c r="AK78">
+        <f t="shared" ref="AK78" si="468">SUM(Q78:Q80)</f>
+        <v>20</v>
+      </c>
+      <c r="AL78">
+        <f t="shared" ref="AL78" si="469">SUM(R78:R80)</f>
+        <v>16</v>
+      </c>
+      <c r="AM78">
+        <f t="shared" ref="AM78" si="470">SUM(S78:S80)</f>
+        <v>3</v>
+      </c>
+      <c r="AN78">
+        <f t="shared" ref="AN78" si="471">SUM(T78:T80)</f>
+        <v>12</v>
+      </c>
+      <c r="AO78">
+        <f t="shared" ref="AO78" si="472">SUM(U78:U80)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>2022</v>
+      </c>
+      <c r="B79" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C79">
+        <v>26</v>
+      </c>
+      <c r="D79" t="s">
+        <v>46</v>
+      </c>
+      <c r="E79" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79">
+        <v>13</v>
+      </c>
+      <c r="G79">
+        <v>4</v>
+      </c>
+      <c r="H79">
+        <v>1</v>
+      </c>
+      <c r="I79" t="s">
+        <v>32</v>
+      </c>
+      <c r="J79" t="s">
+        <v>31</v>
+      </c>
+      <c r="K79">
+        <f t="shared" si="260"/>
+        <v>36</v>
+      </c>
+      <c r="L79">
+        <v>3</v>
+      </c>
+      <c r="M79">
+        <v>5</v>
+      </c>
+      <c r="N79">
+        <v>4</v>
+      </c>
+      <c r="O79">
+        <v>11</v>
+      </c>
+      <c r="P79">
+        <v>5</v>
+      </c>
+      <c r="Q79">
+        <v>6</v>
+      </c>
+      <c r="R79">
+        <v>5</v>
+      </c>
+      <c r="S79">
+        <v>0</v>
+      </c>
+      <c r="T79">
+        <v>5</v>
+      </c>
+      <c r="U79">
+        <v>0</v>
+      </c>
+      <c r="V79">
+        <v>0</v>
+      </c>
+      <c r="W79">
+        <v>0</v>
+      </c>
+      <c r="X79">
+        <v>0</v>
+      </c>
+      <c r="Y79">
+        <v>0</v>
+      </c>
+      <c r="Z79">
+        <v>0</v>
+      </c>
+      <c r="AA79">
+        <v>0</v>
+      </c>
+      <c r="AB79">
+        <v>0</v>
+      </c>
+      <c r="AC79">
+        <v>1</v>
+      </c>
+      <c r="AD79">
+        <v>0</v>
+      </c>
+      <c r="AE79">
+        <v>0</v>
+      </c>
+      <c r="AF79">
+        <v>0</v>
+      </c>
+      <c r="AG79">
+        <v>0</v>
+      </c>
+      <c r="AH79">
+        <f>SUM(N78:N80)</f>
+        <v>9</v>
+      </c>
+      <c r="AI79">
+        <f t="shared" ref="AI79" si="473">SUM(O78:O80)</f>
+        <v>21</v>
+      </c>
+      <c r="AJ79">
+        <f t="shared" ref="AJ79" si="474">SUM(P78:P80)</f>
+        <v>12</v>
+      </c>
+      <c r="AK79">
+        <f t="shared" ref="AK79" si="475">SUM(Q78:Q80)</f>
+        <v>20</v>
+      </c>
+      <c r="AL79">
+        <f t="shared" ref="AL79" si="476">SUM(R78:R80)</f>
+        <v>16</v>
+      </c>
+      <c r="AM79">
+        <f t="shared" ref="AM79" si="477">SUM(S78:S80)</f>
+        <v>3</v>
+      </c>
+      <c r="AN79">
+        <f t="shared" ref="AN79" si="478">SUM(T78:T80)</f>
+        <v>12</v>
+      </c>
+      <c r="AO79">
+        <f t="shared" ref="AO79" si="479">SUM(U78:U80)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>2022</v>
+      </c>
+      <c r="B80" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C80">
+        <v>26</v>
+      </c>
+      <c r="D80" t="s">
+        <v>46</v>
+      </c>
+      <c r="E80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80">
+        <v>8</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>3</v>
+      </c>
+      <c r="I80" t="s">
+        <v>37</v>
+      </c>
+      <c r="J80" t="s">
+        <v>31</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="260"/>
+        <v>31</v>
+      </c>
+      <c r="L80">
+        <v>6</v>
+      </c>
+      <c r="M80">
+        <v>5</v>
+      </c>
+      <c r="N80">
+        <v>2</v>
+      </c>
+      <c r="O80">
+        <v>4</v>
+      </c>
+      <c r="P80">
+        <v>2</v>
+      </c>
+      <c r="Q80">
+        <v>11</v>
+      </c>
+      <c r="R80">
+        <v>5</v>
+      </c>
+      <c r="S80">
+        <v>0</v>
+      </c>
+      <c r="T80">
+        <v>5</v>
+      </c>
+      <c r="U80">
+        <v>2</v>
+      </c>
+      <c r="V80">
+        <v>0</v>
+      </c>
+      <c r="W80">
+        <v>0</v>
+      </c>
+      <c r="X80">
+        <v>0</v>
+      </c>
+      <c r="Y80">
+        <v>0</v>
+      </c>
+      <c r="Z80">
+        <v>0</v>
+      </c>
+      <c r="AA80">
+        <v>0</v>
+      </c>
+      <c r="AB80">
+        <v>0</v>
+      </c>
+      <c r="AC80">
+        <v>0</v>
+      </c>
+      <c r="AD80">
+        <v>0</v>
+      </c>
+      <c r="AE80">
+        <v>0</v>
+      </c>
+      <c r="AF80">
+        <v>0</v>
+      </c>
+      <c r="AG80">
+        <v>0</v>
+      </c>
+      <c r="AH80">
+        <f>SUM(N78:N80)</f>
+        <v>9</v>
+      </c>
+      <c r="AI80">
+        <f t="shared" ref="AI80" si="480">SUM(O78:O80)</f>
+        <v>21</v>
+      </c>
+      <c r="AJ80">
+        <f t="shared" ref="AJ80" si="481">SUM(P78:P80)</f>
+        <v>12</v>
+      </c>
+      <c r="AK80">
+        <f t="shared" ref="AK80" si="482">SUM(Q78:Q80)</f>
+        <v>20</v>
+      </c>
+      <c r="AL80">
+        <f t="shared" ref="AL80" si="483">SUM(R78:R80)</f>
+        <v>16</v>
+      </c>
+      <c r="AM80">
+        <f t="shared" ref="AM80" si="484">SUM(S78:S80)</f>
+        <v>3</v>
+      </c>
+      <c r="AN80">
+        <f t="shared" ref="AN80" si="485">SUM(T78:T80)</f>
+        <v>12</v>
+      </c>
+      <c r="AO80">
+        <f t="shared" ref="AO80" si="486">SUM(U78:U80)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>2022</v>
+      </c>
+      <c r="B81" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C81">
+        <v>27</v>
+      </c>
+      <c r="D81" t="s">
+        <v>46</v>
+      </c>
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81">
+        <v>8</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
+      <c r="H81">
+        <v>2</v>
+      </c>
+      <c r="I81" t="s">
+        <v>36</v>
+      </c>
+      <c r="J81" t="s">
+        <v>31</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="260"/>
+        <v>0</v>
+      </c>
+      <c r="AH81">
+        <f>SUM(N81:N83)</f>
+        <v>0</v>
+      </c>
+      <c r="AI81">
+        <f t="shared" ref="AI81" si="487">SUM(O81:O83)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ81">
+        <f t="shared" ref="AJ81" si="488">SUM(P81:P83)</f>
+        <v>0</v>
+      </c>
+      <c r="AK81">
+        <f t="shared" ref="AK81" si="489">SUM(Q81:Q83)</f>
+        <v>0</v>
+      </c>
+      <c r="AL81">
+        <f t="shared" ref="AL81" si="490">SUM(R81:R83)</f>
+        <v>0</v>
+      </c>
+      <c r="AM81">
+        <f t="shared" ref="AM81" si="491">SUM(S81:S83)</f>
+        <v>0</v>
+      </c>
+      <c r="AN81">
+        <f t="shared" ref="AN81" si="492">SUM(T81:T83)</f>
+        <v>0</v>
+      </c>
+      <c r="AO81">
+        <f t="shared" ref="AO81" si="493">SUM(U81:U83)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>2022</v>
+      </c>
+      <c r="B82" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C82">
+        <v>27</v>
+      </c>
+      <c r="D82" t="s">
+        <v>46</v>
+      </c>
+      <c r="E82" t="s">
+        <v>13</v>
+      </c>
+      <c r="F82">
+        <v>5</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
+        <v>3</v>
+      </c>
+      <c r="I82" t="s">
+        <v>32</v>
+      </c>
+      <c r="J82" t="s">
+        <v>31</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="260"/>
+        <v>0</v>
+      </c>
+      <c r="AH82">
+        <f>SUM(N81:N83)</f>
+        <v>0</v>
+      </c>
+      <c r="AI82">
+        <f t="shared" ref="AI82" si="494">SUM(O81:O83)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ82">
+        <f t="shared" ref="AJ82" si="495">SUM(P81:P83)</f>
+        <v>0</v>
+      </c>
+      <c r="AK82">
+        <f t="shared" ref="AK82" si="496">SUM(Q81:Q83)</f>
+        <v>0</v>
+      </c>
+      <c r="AL82">
+        <f t="shared" ref="AL82" si="497">SUM(R81:R83)</f>
+        <v>0</v>
+      </c>
+      <c r="AM82">
+        <f t="shared" ref="AM82" si="498">SUM(S81:S83)</f>
+        <v>0</v>
+      </c>
+      <c r="AN82">
+        <f t="shared" ref="AN82" si="499">SUM(T81:T83)</f>
+        <v>0</v>
+      </c>
+      <c r="AO82">
+        <f t="shared" ref="AO82" si="500">SUM(U81:U83)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>2022</v>
+      </c>
+      <c r="B83" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C83">
+        <v>27</v>
+      </c>
+      <c r="D83" t="s">
+        <v>46</v>
+      </c>
+      <c r="E83" t="s">
+        <v>12</v>
+      </c>
+      <c r="F83">
+        <v>14</v>
+      </c>
+      <c r="G83">
+        <v>5</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83" t="s">
+        <v>37</v>
+      </c>
+      <c r="J83" t="s">
+        <v>31</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="260"/>
+        <v>0</v>
+      </c>
+      <c r="AH83">
+        <f>SUM(N81:N83)</f>
+        <v>0</v>
+      </c>
+      <c r="AI83">
+        <f t="shared" ref="AI83" si="501">SUM(O81:O83)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ83">
+        <f t="shared" ref="AJ83" si="502">SUM(P81:P83)</f>
+        <v>0</v>
+      </c>
+      <c r="AK83">
+        <f t="shared" ref="AK83" si="503">SUM(Q81:Q83)</f>
+        <v>0</v>
+      </c>
+      <c r="AL83">
+        <f t="shared" ref="AL83" si="504">SUM(R81:R83)</f>
+        <v>0</v>
+      </c>
+      <c r="AM83">
+        <f t="shared" ref="AM83" si="505">SUM(S81:S83)</f>
+        <v>0</v>
+      </c>
+      <c r="AN83">
+        <f t="shared" ref="AN83" si="506">SUM(T81:T83)</f>
+        <v>0</v>
+      </c>
+      <c r="AO83">
+        <f t="shared" ref="AO83" si="507">SUM(U81:U83)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>2022</v>
+      </c>
+      <c r="B84" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C84">
+        <v>28</v>
+      </c>
+      <c r="D84" t="s">
+        <v>46</v>
+      </c>
+      <c r="E84" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84">
+        <v>7</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>3</v>
+      </c>
+      <c r="I84" t="s">
+        <v>36</v>
+      </c>
+      <c r="J84" t="s">
+        <v>31</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="260"/>
+        <v>30</v>
+      </c>
+      <c r="L84">
+        <v>5</v>
+      </c>
+      <c r="M84">
+        <v>5</v>
+      </c>
+      <c r="N84">
+        <v>5</v>
+      </c>
+      <c r="O84">
+        <v>3</v>
+      </c>
+      <c r="P84">
+        <v>3</v>
+      </c>
+      <c r="Q84">
+        <v>12</v>
+      </c>
+      <c r="R84">
+        <v>2</v>
+      </c>
+      <c r="S84">
+        <v>0</v>
+      </c>
+      <c r="T84">
+        <v>2</v>
+      </c>
+      <c r="U84">
+        <v>3</v>
+      </c>
+      <c r="V84">
+        <v>0</v>
+      </c>
+      <c r="W84">
+        <v>0</v>
+      </c>
+      <c r="X84">
+        <v>0</v>
+      </c>
+      <c r="Y84">
+        <v>0</v>
+      </c>
+      <c r="Z84">
+        <v>0</v>
+      </c>
+      <c r="AA84">
+        <v>0</v>
+      </c>
+      <c r="AB84">
+        <v>0</v>
+      </c>
+      <c r="AC84">
+        <v>0</v>
+      </c>
+      <c r="AD84">
+        <v>0</v>
+      </c>
+      <c r="AE84">
+        <v>1</v>
+      </c>
+      <c r="AF84">
+        <v>0</v>
+      </c>
+      <c r="AG84">
+        <v>0</v>
+      </c>
+      <c r="AH84">
+        <f>SUM(N84:N86)</f>
+        <v>17</v>
+      </c>
+      <c r="AI84">
+        <f t="shared" ref="AI84" si="508">SUM(O84:O86)</f>
+        <v>9</v>
+      </c>
+      <c r="AJ84">
+        <f t="shared" ref="AJ84" si="509">SUM(P84:P86)</f>
+        <v>12</v>
+      </c>
+      <c r="AK84">
+        <f t="shared" ref="AK84" si="510">SUM(Q84:Q86)</f>
+        <v>24</v>
+      </c>
+      <c r="AL84">
+        <f t="shared" ref="AL84" si="511">SUM(R84:R86)</f>
+        <v>9</v>
+      </c>
+      <c r="AM84">
+        <f t="shared" ref="AM84" si="512">SUM(S84:S86)</f>
+        <v>10</v>
+      </c>
+      <c r="AN84">
+        <f t="shared" ref="AN84" si="513">SUM(T84:T86)</f>
+        <v>6</v>
+      </c>
+      <c r="AO84">
+        <f t="shared" ref="AO84" si="514">SUM(U84:U86)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>2022</v>
+      </c>
+      <c r="B85" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C85">
+        <v>28</v>
+      </c>
+      <c r="D85" t="s">
+        <v>46</v>
+      </c>
+      <c r="E85" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85">
+        <v>13</v>
+      </c>
+      <c r="G85">
+        <v>6</v>
+      </c>
+      <c r="H85">
+        <v>1</v>
+      </c>
+      <c r="I85" t="s">
+        <v>32</v>
+      </c>
+      <c r="J85" t="s">
+        <v>31</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="260"/>
+        <v>32</v>
+      </c>
+      <c r="L85">
+        <v>6</v>
+      </c>
+      <c r="M85">
+        <v>5</v>
+      </c>
+      <c r="N85">
+        <v>5</v>
+      </c>
+      <c r="O85">
+        <v>3</v>
+      </c>
+      <c r="P85">
+        <v>6</v>
+      </c>
+      <c r="Q85">
+        <v>4</v>
+      </c>
+      <c r="R85">
+        <v>4</v>
+      </c>
+      <c r="S85">
+        <v>5</v>
+      </c>
+      <c r="T85">
+        <v>4</v>
+      </c>
+      <c r="U85">
+        <v>1</v>
+      </c>
+      <c r="V85">
+        <v>0</v>
+      </c>
+      <c r="W85">
+        <v>0</v>
+      </c>
+      <c r="X85">
+        <v>0</v>
+      </c>
+      <c r="Y85">
+        <v>0</v>
+      </c>
+      <c r="Z85">
+        <v>0</v>
+      </c>
+      <c r="AA85">
+        <v>0</v>
+      </c>
+      <c r="AB85">
+        <v>0</v>
+      </c>
+      <c r="AC85">
+        <v>0</v>
+      </c>
+      <c r="AD85">
+        <v>1</v>
+      </c>
+      <c r="AE85">
+        <v>0</v>
+      </c>
+      <c r="AF85">
+        <v>0</v>
+      </c>
+      <c r="AG85">
+        <v>0</v>
+      </c>
+      <c r="AH85">
+        <f>SUM(N84:N86)</f>
+        <v>17</v>
+      </c>
+      <c r="AI85">
+        <f t="shared" ref="AI85" si="515">SUM(O84:O86)</f>
+        <v>9</v>
+      </c>
+      <c r="AJ85">
+        <f t="shared" ref="AJ85" si="516">SUM(P84:P86)</f>
+        <v>12</v>
+      </c>
+      <c r="AK85">
+        <f t="shared" ref="AK85" si="517">SUM(Q84:Q86)</f>
+        <v>24</v>
+      </c>
+      <c r="AL85">
+        <f t="shared" ref="AL85" si="518">SUM(R84:R86)</f>
+        <v>9</v>
+      </c>
+      <c r="AM85">
+        <f t="shared" ref="AM85" si="519">SUM(S84:S86)</f>
+        <v>10</v>
+      </c>
+      <c r="AN85">
+        <f t="shared" ref="AN85" si="520">SUM(T84:T86)</f>
+        <v>6</v>
+      </c>
+      <c r="AO85">
+        <f t="shared" ref="AO85" si="521">SUM(U84:U86)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>2022</v>
+      </c>
+      <c r="B86" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C86">
+        <v>28</v>
+      </c>
+      <c r="D86" t="s">
+        <v>46</v>
+      </c>
+      <c r="E86" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86">
+        <v>10</v>
+      </c>
+      <c r="G86">
+        <v>4</v>
+      </c>
+      <c r="H86">
+        <v>2</v>
+      </c>
+      <c r="I86" t="s">
+        <v>37</v>
+      </c>
+      <c r="J86" t="s">
+        <v>31</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="260"/>
+        <v>32</v>
+      </c>
+      <c r="L86">
+        <v>5</v>
+      </c>
+      <c r="M86">
+        <v>5</v>
+      </c>
+      <c r="N86">
+        <v>7</v>
+      </c>
+      <c r="O86">
+        <v>3</v>
+      </c>
+      <c r="P86">
+        <v>3</v>
+      </c>
+      <c r="Q86">
+        <v>8</v>
+      </c>
+      <c r="R86">
+        <v>3</v>
+      </c>
+      <c r="S86">
+        <v>5</v>
+      </c>
+      <c r="T86">
+        <v>0</v>
+      </c>
+      <c r="U86">
+        <v>3</v>
+      </c>
+      <c r="V86">
+        <v>0</v>
+      </c>
+      <c r="W86">
+        <v>0</v>
+      </c>
+      <c r="X86">
+        <v>0</v>
+      </c>
+      <c r="Y86">
+        <v>0</v>
+      </c>
+      <c r="Z86">
+        <v>0</v>
+      </c>
+      <c r="AA86">
+        <v>0</v>
+      </c>
+      <c r="AB86">
+        <v>0</v>
+      </c>
+      <c r="AC86">
+        <v>1</v>
+      </c>
+      <c r="AD86">
+        <v>0</v>
+      </c>
+      <c r="AE86">
+        <v>0</v>
+      </c>
+      <c r="AF86">
+        <v>0</v>
+      </c>
+      <c r="AG86">
+        <v>0</v>
+      </c>
+      <c r="AH86">
+        <f>SUM(N84:N86)</f>
+        <v>17</v>
+      </c>
+      <c r="AI86">
+        <f t="shared" ref="AI86" si="522">SUM(O84:O86)</f>
+        <v>9</v>
+      </c>
+      <c r="AJ86">
+        <f t="shared" ref="AJ86" si="523">SUM(P84:P86)</f>
+        <v>12</v>
+      </c>
+      <c r="AK86">
+        <f t="shared" ref="AK86" si="524">SUM(Q84:Q86)</f>
+        <v>24</v>
+      </c>
+      <c r="AL86">
+        <f t="shared" ref="AL86" si="525">SUM(R84:R86)</f>
+        <v>9</v>
+      </c>
+      <c r="AM86">
+        <f t="shared" ref="AM86" si="526">SUM(S84:S86)</f>
+        <v>10</v>
+      </c>
+      <c r="AN86">
+        <f t="shared" ref="AN86" si="527">SUM(T84:T86)</f>
+        <v>6</v>
+      </c>
+      <c r="AO86">
+        <f t="shared" ref="AO86" si="528">SUM(U84:U86)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>2022</v>
+      </c>
+      <c r="B87" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C87">
+        <v>29</v>
+      </c>
+      <c r="D87" t="s">
+        <v>46</v>
+      </c>
+      <c r="E87" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87">
+        <v>8</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>3</v>
+      </c>
+      <c r="I87" t="s">
+        <v>36</v>
+      </c>
+      <c r="J87" t="s">
+        <v>31</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="260"/>
+        <v>28</v>
+      </c>
+      <c r="L87">
+        <v>4</v>
+      </c>
+      <c r="M87">
+        <v>4</v>
+      </c>
+      <c r="N87">
+        <v>3</v>
+      </c>
+      <c r="O87">
+        <v>15</v>
+      </c>
+      <c r="P87">
+        <v>3</v>
+      </c>
+      <c r="Q87">
+        <v>0</v>
+      </c>
+      <c r="R87">
+        <v>4</v>
+      </c>
+      <c r="S87">
+        <v>3</v>
+      </c>
+      <c r="T87">
+        <v>0</v>
+      </c>
+      <c r="U87">
+        <v>0</v>
+      </c>
+      <c r="V87">
+        <v>0</v>
+      </c>
+      <c r="W87">
+        <v>0</v>
+      </c>
+      <c r="X87">
+        <v>0</v>
+      </c>
+      <c r="Y87">
+        <v>0</v>
+      </c>
+      <c r="Z87">
+        <v>0</v>
+      </c>
+      <c r="AA87">
+        <v>1</v>
+      </c>
+      <c r="AB87">
+        <v>0</v>
+      </c>
+      <c r="AC87">
+        <v>0</v>
+      </c>
+      <c r="AD87">
+        <v>0</v>
+      </c>
+      <c r="AE87">
+        <v>0</v>
+      </c>
+      <c r="AF87">
+        <v>1</v>
+      </c>
+      <c r="AG87">
+        <v>0</v>
+      </c>
+      <c r="AH87">
+        <f>SUM(N87:N89)</f>
+        <v>16</v>
+      </c>
+      <c r="AI87">
+        <f t="shared" ref="AI87" si="529">SUM(O87:O89)</f>
+        <v>20</v>
+      </c>
+      <c r="AJ87">
+        <f t="shared" ref="AJ87" si="530">SUM(P87:P89)</f>
+        <v>11</v>
+      </c>
+      <c r="AK87">
+        <f t="shared" ref="AK87" si="531">SUM(Q87:Q89)</f>
+        <v>12</v>
+      </c>
+      <c r="AL87">
+        <f t="shared" ref="AL87" si="532">SUM(R87:R89)</f>
+        <v>10</v>
+      </c>
+      <c r="AM87">
+        <f t="shared" ref="AM87" si="533">SUM(S87:S89)</f>
+        <v>16</v>
+      </c>
+      <c r="AN87">
+        <f t="shared" ref="AN87" si="534">SUM(T87:T89)</f>
+        <v>4</v>
+      </c>
+      <c r="AO87">
+        <f t="shared" ref="AO87" si="535">SUM(U87:U89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>2022</v>
+      </c>
+      <c r="B88" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C88">
+        <v>29</v>
+      </c>
+      <c r="D88" t="s">
+        <v>46</v>
+      </c>
+      <c r="E88" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88">
+        <v>9</v>
+      </c>
+      <c r="G88">
+        <v>4</v>
+      </c>
+      <c r="H88">
+        <v>2</v>
+      </c>
+      <c r="I88" t="s">
+        <v>32</v>
+      </c>
+      <c r="J88" t="s">
+        <v>31</v>
+      </c>
+      <c r="K88">
+        <f t="shared" si="260"/>
+        <v>27</v>
+      </c>
+      <c r="L88">
+        <v>6</v>
+      </c>
+      <c r="M88">
+        <v>4</v>
+      </c>
+      <c r="N88">
+        <v>6</v>
+      </c>
+      <c r="O88">
+        <v>5</v>
+      </c>
+      <c r="P88">
+        <v>0</v>
+      </c>
+      <c r="Q88">
+        <v>8</v>
+      </c>
+      <c r="R88">
+        <v>2</v>
+      </c>
+      <c r="S88">
+        <v>6</v>
+      </c>
+      <c r="T88">
+        <v>0</v>
+      </c>
+      <c r="U88">
+        <v>0</v>
+      </c>
+      <c r="V88">
+        <v>0</v>
+      </c>
+      <c r="W88">
+        <v>0</v>
+      </c>
+      <c r="X88">
+        <v>0</v>
+      </c>
+      <c r="Y88">
+        <v>0</v>
+      </c>
+      <c r="Z88">
+        <v>0</v>
+      </c>
+      <c r="AA88">
+        <v>0</v>
+      </c>
+      <c r="AB88">
+        <v>0</v>
+      </c>
+      <c r="AC88">
+        <v>0</v>
+      </c>
+      <c r="AD88">
+        <v>0</v>
+      </c>
+      <c r="AE88">
+        <v>0</v>
+      </c>
+      <c r="AF88">
+        <v>0</v>
+      </c>
+      <c r="AG88">
+        <v>1</v>
+      </c>
+      <c r="AH88">
+        <f>SUM(N87:N89)</f>
+        <v>16</v>
+      </c>
+      <c r="AI88">
+        <f t="shared" ref="AI88" si="536">SUM(O87:O89)</f>
+        <v>20</v>
+      </c>
+      <c r="AJ88">
+        <f t="shared" ref="AJ88" si="537">SUM(P87:P89)</f>
+        <v>11</v>
+      </c>
+      <c r="AK88">
+        <f t="shared" ref="AK88" si="538">SUM(Q87:Q89)</f>
+        <v>12</v>
+      </c>
+      <c r="AL88">
+        <f t="shared" ref="AL88" si="539">SUM(R87:R89)</f>
+        <v>10</v>
+      </c>
+      <c r="AM88">
+        <f t="shared" ref="AM88" si="540">SUM(S87:S89)</f>
+        <v>16</v>
+      </c>
+      <c r="AN88">
+        <f t="shared" ref="AN88" si="541">SUM(T87:T89)</f>
+        <v>4</v>
+      </c>
+      <c r="AO88">
+        <f t="shared" ref="AO88" si="542">SUM(U87:U89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>2022</v>
+      </c>
+      <c r="B89" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C89">
+        <v>29</v>
+      </c>
+      <c r="D89" t="s">
+        <v>46</v>
+      </c>
+      <c r="E89" t="s">
+        <v>13</v>
+      </c>
+      <c r="F89">
+        <v>13</v>
+      </c>
+      <c r="G89">
+        <v>7</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="I89" t="s">
+        <v>37</v>
+      </c>
+      <c r="J89" t="s">
+        <v>31</v>
+      </c>
+      <c r="K89">
+        <f t="shared" si="260"/>
+        <v>34</v>
+      </c>
+      <c r="L89">
+        <v>5</v>
+      </c>
+      <c r="M89">
+        <v>4</v>
+      </c>
+      <c r="N89">
+        <v>7</v>
+      </c>
+      <c r="O89">
+        <v>0</v>
+      </c>
+      <c r="P89">
+        <v>8</v>
+      </c>
+      <c r="Q89">
+        <v>4</v>
+      </c>
+      <c r="R89">
+        <v>4</v>
+      </c>
+      <c r="S89">
+        <v>7</v>
+      </c>
+      <c r="T89">
+        <v>4</v>
+      </c>
+      <c r="U89">
+        <v>0</v>
+      </c>
+      <c r="V89">
+        <v>0</v>
+      </c>
+      <c r="W89">
+        <v>0</v>
+      </c>
+      <c r="X89">
+        <v>0</v>
+      </c>
+      <c r="Y89">
+        <v>0</v>
+      </c>
+      <c r="Z89">
+        <v>0</v>
+      </c>
+      <c r="AA89">
+        <v>0</v>
+      </c>
+      <c r="AB89">
+        <v>0</v>
+      </c>
+      <c r="AC89">
+        <v>0</v>
+      </c>
+      <c r="AD89">
+        <v>1</v>
+      </c>
+      <c r="AE89">
+        <v>1</v>
+      </c>
+      <c r="AF89">
+        <v>0</v>
+      </c>
+      <c r="AG89">
+        <v>0</v>
+      </c>
+      <c r="AH89">
+        <f>SUM(N87:N89)</f>
+        <v>16</v>
+      </c>
+      <c r="AI89">
+        <f t="shared" ref="AI89" si="543">SUM(O87:O89)</f>
+        <v>20</v>
+      </c>
+      <c r="AJ89">
+        <f t="shared" ref="AJ89" si="544">SUM(P87:P89)</f>
+        <v>11</v>
+      </c>
+      <c r="AK89">
+        <f t="shared" ref="AK89" si="545">SUM(Q87:Q89)</f>
+        <v>12</v>
+      </c>
+      <c r="AL89">
+        <f t="shared" ref="AL89" si="546">SUM(R87:R89)</f>
+        <v>10</v>
+      </c>
+      <c r="AM89">
+        <f t="shared" ref="AM89" si="547">SUM(S87:S89)</f>
+        <v>16</v>
+      </c>
+      <c r="AN89">
+        <f t="shared" ref="AN89" si="548">SUM(T87:T89)</f>
+        <v>4</v>
+      </c>
+      <c r="AO89">
+        <f t="shared" ref="AO89" si="549">SUM(U87:U89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>2022</v>
+      </c>
+      <c r="B90" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C90">
+        <v>30</v>
+      </c>
+      <c r="D90" t="s">
+        <v>46</v>
+      </c>
+      <c r="E90" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90">
+        <v>13</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>1</v>
+      </c>
+      <c r="I90" t="s">
+        <v>36</v>
+      </c>
+      <c r="J90" t="s">
+        <v>31</v>
+      </c>
+      <c r="K90">
+        <f t="shared" si="260"/>
+        <v>33</v>
+      </c>
+      <c r="L90">
+        <v>6</v>
+      </c>
+      <c r="M90">
+        <v>5</v>
+      </c>
+      <c r="N90">
+        <v>5</v>
+      </c>
+      <c r="O90">
+        <v>4</v>
+      </c>
+      <c r="P90">
+        <v>5</v>
+      </c>
+      <c r="Q90">
+        <v>4</v>
+      </c>
+      <c r="R90">
+        <v>5</v>
+      </c>
+      <c r="S90">
+        <v>5</v>
+      </c>
+      <c r="T90">
+        <v>0</v>
+      </c>
+      <c r="U90">
+        <v>5</v>
+      </c>
+      <c r="V90">
+        <v>0</v>
+      </c>
+      <c r="W90">
+        <v>0</v>
+      </c>
+      <c r="X90">
+        <v>0</v>
+      </c>
+      <c r="Y90">
+        <v>0</v>
+      </c>
+      <c r="Z90">
+        <v>0</v>
+      </c>
+      <c r="AA90">
+        <v>0</v>
+      </c>
+      <c r="AB90">
+        <v>0</v>
+      </c>
+      <c r="AC90">
+        <v>0</v>
+      </c>
+      <c r="AD90">
+        <v>1</v>
+      </c>
+      <c r="AE90">
+        <v>0</v>
+      </c>
+      <c r="AF90">
+        <v>1</v>
+      </c>
+      <c r="AG90">
+        <v>0</v>
+      </c>
+      <c r="AH90">
+        <f>SUM(N90:N92)</f>
+        <v>20</v>
+      </c>
+      <c r="AI90">
+        <f t="shared" ref="AI90" si="550">SUM(O90:O92)</f>
+        <v>12</v>
+      </c>
+      <c r="AJ90">
+        <f t="shared" ref="AJ90" si="551">SUM(P90:P92)</f>
+        <v>16</v>
+      </c>
+      <c r="AK90">
+        <f t="shared" ref="AK90" si="552">SUM(Q90:Q92)</f>
+        <v>8</v>
+      </c>
+      <c r="AL90">
+        <f t="shared" ref="AL90" si="553">SUM(R90:R92)</f>
+        <v>13</v>
+      </c>
+      <c r="AM90">
+        <f t="shared" ref="AM90" si="554">SUM(S90:S92)</f>
+        <v>20</v>
+      </c>
+      <c r="AN90">
+        <f t="shared" ref="AN90" si="555">SUM(T90:T92)</f>
+        <v>0</v>
+      </c>
+      <c r="AO90">
+        <f t="shared" ref="AO90" si="556">SUM(U90:U92)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>2022</v>
+      </c>
+      <c r="B91" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C91">
+        <v>30</v>
+      </c>
+      <c r="D91" t="s">
+        <v>46</v>
+      </c>
+      <c r="E91" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91">
+        <v>10</v>
+      </c>
+      <c r="G91">
+        <v>4</v>
+      </c>
+      <c r="H91">
+        <v>3</v>
+      </c>
+      <c r="I91" t="s">
+        <v>32</v>
+      </c>
+      <c r="J91" t="s">
+        <v>31</v>
+      </c>
+      <c r="K91">
+        <f t="shared" si="260"/>
+        <v>31</v>
+      </c>
+      <c r="L91">
+        <v>6</v>
+      </c>
+      <c r="M91">
+        <v>5</v>
+      </c>
+      <c r="N91">
+        <v>3</v>
+      </c>
+      <c r="O91">
+        <v>8</v>
+      </c>
+      <c r="P91">
+        <v>8</v>
+      </c>
+      <c r="Q91">
+        <v>2</v>
+      </c>
+      <c r="R91">
+        <v>4</v>
+      </c>
+      <c r="S91">
+        <v>3</v>
+      </c>
+      <c r="T91">
+        <v>0</v>
+      </c>
+      <c r="U91">
+        <v>3</v>
+      </c>
+      <c r="V91">
+        <v>0</v>
+      </c>
+      <c r="W91">
+        <v>0</v>
+      </c>
+      <c r="X91">
+        <v>0</v>
+      </c>
+      <c r="Y91">
+        <v>0</v>
+      </c>
+      <c r="Z91">
+        <v>0</v>
+      </c>
+      <c r="AA91">
+        <v>0</v>
+      </c>
+      <c r="AB91">
+        <v>0</v>
+      </c>
+      <c r="AC91">
+        <v>1</v>
+      </c>
+      <c r="AD91">
+        <v>0</v>
+      </c>
+      <c r="AE91">
+        <v>0</v>
+      </c>
+      <c r="AF91">
+        <v>0</v>
+      </c>
+      <c r="AG91">
+        <v>0</v>
+      </c>
+      <c r="AH91">
+        <f>SUM(N90:N92)</f>
+        <v>20</v>
+      </c>
+      <c r="AI91">
+        <f t="shared" ref="AI91" si="557">SUM(O90:O92)</f>
+        <v>12</v>
+      </c>
+      <c r="AJ91">
+        <f t="shared" ref="AJ91" si="558">SUM(P90:P92)</f>
+        <v>16</v>
+      </c>
+      <c r="AK91">
+        <f t="shared" ref="AK91" si="559">SUM(Q90:Q92)</f>
+        <v>8</v>
+      </c>
+      <c r="AL91">
+        <f t="shared" ref="AL91" si="560">SUM(R90:R92)</f>
+        <v>13</v>
+      </c>
+      <c r="AM91">
+        <f t="shared" ref="AM91" si="561">SUM(S90:S92)</f>
+        <v>20</v>
+      </c>
+      <c r="AN91">
+        <f t="shared" ref="AN91" si="562">SUM(T90:T92)</f>
+        <v>0</v>
+      </c>
+      <c r="AO91">
+        <f t="shared" ref="AO91" si="563">SUM(U90:U92)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>2022</v>
+      </c>
+      <c r="B92" s="5">
+        <v>44924</v>
+      </c>
+      <c r="C92">
+        <v>30</v>
+      </c>
+      <c r="D92" t="s">
+        <v>46</v>
+      </c>
+      <c r="E92" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92">
+        <v>11</v>
+      </c>
+      <c r="G92">
+        <v>4</v>
+      </c>
+      <c r="H92">
+        <v>2</v>
+      </c>
+      <c r="I92" t="s">
+        <v>37</v>
+      </c>
+      <c r="J92" t="s">
+        <v>31</v>
+      </c>
+      <c r="K92">
+        <f t="shared" si="260"/>
+        <v>33</v>
+      </c>
+      <c r="L92">
+        <v>6</v>
+      </c>
+      <c r="M92">
+        <v>4</v>
+      </c>
+      <c r="N92">
+        <v>12</v>
+      </c>
+      <c r="O92">
+        <v>0</v>
+      </c>
+      <c r="P92">
+        <v>3</v>
+      </c>
+      <c r="Q92">
+        <v>2</v>
+      </c>
+      <c r="R92">
+        <v>4</v>
+      </c>
+      <c r="S92">
+        <v>12</v>
+      </c>
+      <c r="T92">
+        <v>0</v>
+      </c>
+      <c r="U92">
+        <v>0</v>
+      </c>
+      <c r="V92">
+        <v>0</v>
+      </c>
+      <c r="W92">
+        <v>0</v>
+      </c>
+      <c r="X92">
+        <v>0</v>
+      </c>
+      <c r="Y92">
+        <v>0</v>
+      </c>
+      <c r="Z92">
+        <v>0</v>
+      </c>
+      <c r="AA92">
+        <v>0</v>
+      </c>
+      <c r="AB92">
+        <v>0</v>
+      </c>
+      <c r="AC92">
+        <v>0</v>
+      </c>
+      <c r="AD92">
+        <v>0</v>
+      </c>
+      <c r="AE92">
+        <v>0</v>
+      </c>
+      <c r="AF92">
+        <v>0</v>
+      </c>
+      <c r="AG92">
+        <v>1</v>
+      </c>
+      <c r="AH92">
+        <f>SUM(N90:N92)</f>
+        <v>20</v>
+      </c>
+      <c r="AI92">
+        <f t="shared" ref="AI92" si="564">SUM(O90:O92)</f>
+        <v>12</v>
+      </c>
+      <c r="AJ92">
+        <f t="shared" ref="AJ92" si="565">SUM(P90:P92)</f>
+        <v>16</v>
+      </c>
+      <c r="AK92">
+        <f t="shared" ref="AK92" si="566">SUM(Q90:Q92)</f>
+        <v>8</v>
+      </c>
+      <c r="AL92">
+        <f t="shared" ref="AL92" si="567">SUM(R90:R92)</f>
+        <v>13</v>
+      </c>
+      <c r="AM92">
+        <f t="shared" ref="AM92" si="568">SUM(S90:S92)</f>
+        <v>20</v>
+      </c>
+      <c r="AN92">
+        <f t="shared" ref="AN92" si="569">SUM(T90:T92)</f>
+        <v>0</v>
+      </c>
+      <c r="AO92">
+        <f t="shared" ref="AO92" si="570">SUM(U90:U92)</f>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data update 2024 finale
</commit_message>
<xml_diff>
--- a/catan_data.xlsx
+++ b/catan_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/88b1f18c208c1b3c/Documents/CatanData/catan_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfu\OneDrive\Documents\CatanData\catan_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{EC8D8D10-CA15-4B3B-8470-61355121DCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D04FB61F-DEFB-45A2-880B-78B00A63E26A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A0C7DD-2B7E-487B-9B32-F6E167B7ECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{83B30B11-FE95-4925-9DB4-CCB67C570BD6}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AP$272</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AP$290</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="71">
   <si>
     <t>season</t>
   </si>
@@ -628,13 +628,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8635BA-0A9D-4832-9FDC-B5CDD32D9D6C}">
-  <dimension ref="A1:AP275"/>
+  <dimension ref="A1:AP293"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="9" ySplit="2" topLeftCell="J249" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="2" topLeftCell="J272" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B275" sqref="B275"/>
+      <selection pane="bottomRight" activeCell="E288" sqref="E288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3320,7 +3320,7 @@
         <v>11</v>
       </c>
       <c r="G27">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H27">
         <v>5</v>
@@ -18273,7 +18273,7 @@
         <v>11</v>
       </c>
       <c r="G172">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H172">
         <v>7</v>
@@ -26458,7 +26458,7 @@
         <v>31</v>
       </c>
       <c r="L251">
-        <f t="shared" ref="L251:L275" si="5">SUM(O251:V251)</f>
+        <f t="shared" ref="L251:L293" si="5">SUM(O251:V251)</f>
         <v>34</v>
       </c>
       <c r="M251">
@@ -27157,7 +27157,7 @@
         <v>11</v>
       </c>
       <c r="G258">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H258">
         <v>8</v>
@@ -28976,8 +28976,1844 @@
         <v>0</v>
       </c>
     </row>
+    <row r="276" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A276">
+        <v>2024</v>
+      </c>
+      <c r="B276" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C276">
+        <v>40</v>
+      </c>
+      <c r="D276" t="s">
+        <v>46</v>
+      </c>
+      <c r="F276" t="s">
+        <v>12</v>
+      </c>
+      <c r="G276">
+        <v>8</v>
+      </c>
+      <c r="H276">
+        <v>2</v>
+      </c>
+      <c r="I276">
+        <v>3</v>
+      </c>
+      <c r="J276" t="s">
+        <v>36</v>
+      </c>
+      <c r="K276" t="s">
+        <v>31</v>
+      </c>
+      <c r="L276">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="M276">
+        <v>5</v>
+      </c>
+      <c r="N276">
+        <v>4</v>
+      </c>
+      <c r="O276">
+        <v>5</v>
+      </c>
+      <c r="P276">
+        <v>0</v>
+      </c>
+      <c r="Q276">
+        <v>3</v>
+      </c>
+      <c r="R276">
+        <v>5</v>
+      </c>
+      <c r="S276">
+        <v>8</v>
+      </c>
+      <c r="T276">
+        <v>2</v>
+      </c>
+      <c r="U276">
+        <v>4</v>
+      </c>
+      <c r="V276">
+        <v>4</v>
+      </c>
+      <c r="W276">
+        <v>0</v>
+      </c>
+      <c r="X276">
+        <v>0</v>
+      </c>
+      <c r="Y276">
+        <v>0</v>
+      </c>
+      <c r="Z276">
+        <v>0</v>
+      </c>
+      <c r="AA276">
+        <v>0</v>
+      </c>
+      <c r="AB276">
+        <v>0</v>
+      </c>
+      <c r="AC276">
+        <v>0</v>
+      </c>
+      <c r="AD276">
+        <v>0</v>
+      </c>
+      <c r="AE276">
+        <v>0</v>
+      </c>
+      <c r="AF276">
+        <v>0</v>
+      </c>
+      <c r="AG276">
+        <v>1</v>
+      </c>
+      <c r="AH276">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A277">
+        <v>2024</v>
+      </c>
+      <c r="B277" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C277">
+        <v>40</v>
+      </c>
+      <c r="D277" t="s">
+        <v>46</v>
+      </c>
+      <c r="F277" t="s">
+        <v>11</v>
+      </c>
+      <c r="G277">
+        <v>10</v>
+      </c>
+      <c r="H277">
+        <v>2</v>
+      </c>
+      <c r="I277">
+        <v>2</v>
+      </c>
+      <c r="J277" t="s">
+        <v>32</v>
+      </c>
+      <c r="K277" t="s">
+        <v>31</v>
+      </c>
+      <c r="L277">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="M277">
+        <v>6</v>
+      </c>
+      <c r="N277">
+        <v>4</v>
+      </c>
+      <c r="O277">
+        <v>5</v>
+      </c>
+      <c r="P277">
+        <v>17</v>
+      </c>
+      <c r="Q277">
+        <v>4</v>
+      </c>
+      <c r="R277">
+        <v>0</v>
+      </c>
+      <c r="S277">
+        <v>1</v>
+      </c>
+      <c r="T277">
+        <v>0</v>
+      </c>
+      <c r="U277">
+        <v>1</v>
+      </c>
+      <c r="V277">
+        <v>4</v>
+      </c>
+      <c r="W277">
+        <v>0</v>
+      </c>
+      <c r="X277">
+        <v>0</v>
+      </c>
+      <c r="Y277">
+        <v>0</v>
+      </c>
+      <c r="Z277">
+        <v>0</v>
+      </c>
+      <c r="AA277">
+        <v>0</v>
+      </c>
+      <c r="AB277">
+        <v>0</v>
+      </c>
+      <c r="AC277">
+        <v>0</v>
+      </c>
+      <c r="AD277">
+        <v>1</v>
+      </c>
+      <c r="AE277">
+        <v>0</v>
+      </c>
+      <c r="AF277">
+        <v>0</v>
+      </c>
+      <c r="AG277">
+        <v>0</v>
+      </c>
+      <c r="AH277">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A278">
+        <v>2024</v>
+      </c>
+      <c r="B278" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C278">
+        <v>40</v>
+      </c>
+      <c r="D278" t="s">
+        <v>46</v>
+      </c>
+      <c r="F278" t="s">
+        <v>13</v>
+      </c>
+      <c r="G278">
+        <v>13</v>
+      </c>
+      <c r="H278">
+        <v>5</v>
+      </c>
+      <c r="I278">
+        <v>1</v>
+      </c>
+      <c r="J278" t="s">
+        <v>37</v>
+      </c>
+      <c r="K278" t="s">
+        <v>31</v>
+      </c>
+      <c r="L278">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="M278">
+        <v>6</v>
+      </c>
+      <c r="N278">
+        <v>5</v>
+      </c>
+      <c r="O278">
+        <v>2</v>
+      </c>
+      <c r="P278">
+        <v>3</v>
+      </c>
+      <c r="Q278">
+        <v>5</v>
+      </c>
+      <c r="R278">
+        <v>2</v>
+      </c>
+      <c r="S278">
+        <v>8</v>
+      </c>
+      <c r="T278">
+        <v>0</v>
+      </c>
+      <c r="U278">
+        <v>8</v>
+      </c>
+      <c r="V278">
+        <v>5</v>
+      </c>
+      <c r="W278">
+        <v>0</v>
+      </c>
+      <c r="X278">
+        <v>0</v>
+      </c>
+      <c r="Y278">
+        <v>0</v>
+      </c>
+      <c r="Z278">
+        <v>0</v>
+      </c>
+      <c r="AA278">
+        <v>0</v>
+      </c>
+      <c r="AB278">
+        <v>0</v>
+      </c>
+      <c r="AC278">
+        <v>0</v>
+      </c>
+      <c r="AD278">
+        <v>0</v>
+      </c>
+      <c r="AE278">
+        <v>0</v>
+      </c>
+      <c r="AF278">
+        <v>0</v>
+      </c>
+      <c r="AG278">
+        <v>1</v>
+      </c>
+      <c r="AH278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A279">
+        <v>2024</v>
+      </c>
+      <c r="B279" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C279">
+        <v>41</v>
+      </c>
+      <c r="D279" t="s">
+        <v>46</v>
+      </c>
+      <c r="F279" t="s">
+        <v>11</v>
+      </c>
+      <c r="G279">
+        <v>12</v>
+      </c>
+      <c r="H279">
+        <v>3</v>
+      </c>
+      <c r="I279">
+        <v>2</v>
+      </c>
+      <c r="J279" t="s">
+        <v>36</v>
+      </c>
+      <c r="K279" t="s">
+        <v>31</v>
+      </c>
+      <c r="L279">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="M279">
+        <v>6</v>
+      </c>
+      <c r="N279">
+        <v>5</v>
+      </c>
+      <c r="O279">
+        <v>5</v>
+      </c>
+      <c r="P279">
+        <v>6</v>
+      </c>
+      <c r="Q279">
+        <v>5</v>
+      </c>
+      <c r="R279">
+        <v>9</v>
+      </c>
+      <c r="S279">
+        <v>4</v>
+      </c>
+      <c r="T279">
+        <v>5</v>
+      </c>
+      <c r="U279">
+        <v>0</v>
+      </c>
+      <c r="V279">
+        <v>0</v>
+      </c>
+      <c r="W279">
+        <v>0</v>
+      </c>
+      <c r="X279">
+        <v>0</v>
+      </c>
+      <c r="Y279">
+        <v>0</v>
+      </c>
+      <c r="Z279">
+        <v>0</v>
+      </c>
+      <c r="AA279">
+        <v>0</v>
+      </c>
+      <c r="AB279">
+        <v>0</v>
+      </c>
+      <c r="AC279">
+        <v>0</v>
+      </c>
+      <c r="AD279">
+        <v>0</v>
+      </c>
+      <c r="AE279">
+        <v>0</v>
+      </c>
+      <c r="AF279">
+        <v>0</v>
+      </c>
+      <c r="AG279">
+        <v>0</v>
+      </c>
+      <c r="AH279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A280">
+        <v>2024</v>
+      </c>
+      <c r="B280" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C280">
+        <v>41</v>
+      </c>
+      <c r="D280" t="s">
+        <v>46</v>
+      </c>
+      <c r="F280" t="s">
+        <v>12</v>
+      </c>
+      <c r="G280">
+        <v>9</v>
+      </c>
+      <c r="H280">
+        <v>2</v>
+      </c>
+      <c r="I280">
+        <v>3</v>
+      </c>
+      <c r="J280" t="s">
+        <v>32</v>
+      </c>
+      <c r="K280" t="s">
+        <v>31</v>
+      </c>
+      <c r="L280">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="M280">
+        <v>6</v>
+      </c>
+      <c r="N280">
+        <v>5</v>
+      </c>
+      <c r="O280">
+        <v>4</v>
+      </c>
+      <c r="P280">
+        <v>6</v>
+      </c>
+      <c r="Q280">
+        <v>3</v>
+      </c>
+      <c r="R280">
+        <v>5</v>
+      </c>
+      <c r="S280">
+        <v>9</v>
+      </c>
+      <c r="T280">
+        <v>0</v>
+      </c>
+      <c r="U280">
+        <v>9</v>
+      </c>
+      <c r="V280">
+        <v>0</v>
+      </c>
+      <c r="W280">
+        <v>0</v>
+      </c>
+      <c r="X280">
+        <v>0</v>
+      </c>
+      <c r="Y280">
+        <v>0</v>
+      </c>
+      <c r="Z280">
+        <v>0</v>
+      </c>
+      <c r="AA280">
+        <v>0</v>
+      </c>
+      <c r="AB280">
+        <v>0</v>
+      </c>
+      <c r="AC280">
+        <v>0</v>
+      </c>
+      <c r="AD280">
+        <v>0</v>
+      </c>
+      <c r="AE280">
+        <v>0</v>
+      </c>
+      <c r="AF280">
+        <v>0</v>
+      </c>
+      <c r="AG280">
+        <v>0</v>
+      </c>
+      <c r="AH280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A281">
+        <v>2024</v>
+      </c>
+      <c r="B281" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C281">
+        <v>41</v>
+      </c>
+      <c r="D281" t="s">
+        <v>46</v>
+      </c>
+      <c r="F281" t="s">
+        <v>13</v>
+      </c>
+      <c r="G281">
+        <v>13</v>
+      </c>
+      <c r="H281">
+        <v>5</v>
+      </c>
+      <c r="I281">
+        <v>1</v>
+      </c>
+      <c r="J281" t="s">
+        <v>37</v>
+      </c>
+      <c r="K281" t="s">
+        <v>31</v>
+      </c>
+      <c r="L281">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="M281">
+        <v>5</v>
+      </c>
+      <c r="N281">
+        <v>5</v>
+      </c>
+      <c r="O281">
+        <v>3</v>
+      </c>
+      <c r="P281">
+        <v>3</v>
+      </c>
+      <c r="Q281">
+        <v>5</v>
+      </c>
+      <c r="R281">
+        <v>7</v>
+      </c>
+      <c r="S281">
+        <v>4</v>
+      </c>
+      <c r="T281">
+        <v>3</v>
+      </c>
+      <c r="U281">
+        <v>4</v>
+      </c>
+      <c r="V281">
+        <v>5</v>
+      </c>
+      <c r="W281">
+        <v>0</v>
+      </c>
+      <c r="X281">
+        <v>0</v>
+      </c>
+      <c r="Y281">
+        <v>0</v>
+      </c>
+      <c r="Z281">
+        <v>0</v>
+      </c>
+      <c r="AA281">
+        <v>0</v>
+      </c>
+      <c r="AB281">
+        <v>0</v>
+      </c>
+      <c r="AC281">
+        <v>0</v>
+      </c>
+      <c r="AD281">
+        <v>1</v>
+      </c>
+      <c r="AE281">
+        <v>1</v>
+      </c>
+      <c r="AF281">
+        <v>0</v>
+      </c>
+      <c r="AG281">
+        <v>0</v>
+      </c>
+      <c r="AH281">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="282" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A282">
+        <v>2024</v>
+      </c>
+      <c r="B282" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C282">
+        <v>42</v>
+      </c>
+      <c r="D282" t="s">
+        <v>46</v>
+      </c>
+      <c r="F282" t="s">
+        <v>12</v>
+      </c>
+      <c r="G282">
+        <v>13</v>
+      </c>
+      <c r="H282">
+        <v>6</v>
+      </c>
+      <c r="I282">
+        <v>1</v>
+      </c>
+      <c r="J282" t="s">
+        <v>36</v>
+      </c>
+      <c r="K282" t="s">
+        <v>31</v>
+      </c>
+      <c r="L282">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="M282">
+        <v>5</v>
+      </c>
+      <c r="N282">
+        <v>4</v>
+      </c>
+      <c r="O282">
+        <v>3</v>
+      </c>
+      <c r="P282">
+        <v>22</v>
+      </c>
+      <c r="Q282">
+        <v>0</v>
+      </c>
+      <c r="R282">
+        <v>4</v>
+      </c>
+      <c r="S282">
+        <v>5</v>
+      </c>
+      <c r="T282">
+        <v>0</v>
+      </c>
+      <c r="U282">
+        <v>0</v>
+      </c>
+      <c r="V282">
+        <v>0</v>
+      </c>
+      <c r="W282">
+        <v>0</v>
+      </c>
+      <c r="X282">
+        <v>0</v>
+      </c>
+      <c r="Y282">
+        <v>0</v>
+      </c>
+      <c r="Z282">
+        <v>0</v>
+      </c>
+      <c r="AA282">
+        <v>0</v>
+      </c>
+      <c r="AB282">
+        <v>0</v>
+      </c>
+      <c r="AC282">
+        <v>0</v>
+      </c>
+      <c r="AD282">
+        <v>0</v>
+      </c>
+      <c r="AE282">
+        <v>0</v>
+      </c>
+      <c r="AF282">
+        <v>0</v>
+      </c>
+      <c r="AG282">
+        <v>0</v>
+      </c>
+      <c r="AH282">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="283" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A283">
+        <v>2024</v>
+      </c>
+      <c r="B283" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C283">
+        <v>42</v>
+      </c>
+      <c r="D283" t="s">
+        <v>46</v>
+      </c>
+      <c r="F283" t="s">
+        <v>11</v>
+      </c>
+      <c r="G283">
+        <v>7</v>
+      </c>
+      <c r="H283">
+        <v>2</v>
+      </c>
+      <c r="I283">
+        <v>2</v>
+      </c>
+      <c r="J283" t="s">
+        <v>32</v>
+      </c>
+      <c r="K283" t="s">
+        <v>31</v>
+      </c>
+      <c r="L283">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="M283">
+        <v>6</v>
+      </c>
+      <c r="N283">
+        <v>4</v>
+      </c>
+      <c r="O283">
+        <v>5</v>
+      </c>
+      <c r="P283">
+        <v>0</v>
+      </c>
+      <c r="Q283">
+        <v>5</v>
+      </c>
+      <c r="R283">
+        <v>3</v>
+      </c>
+      <c r="S283">
+        <v>9</v>
+      </c>
+      <c r="T283">
+        <v>1</v>
+      </c>
+      <c r="U283">
+        <v>9</v>
+      </c>
+      <c r="V283">
+        <v>0</v>
+      </c>
+      <c r="W283">
+        <v>0</v>
+      </c>
+      <c r="X283">
+        <v>0</v>
+      </c>
+      <c r="Y283">
+        <v>0</v>
+      </c>
+      <c r="Z283">
+        <v>0</v>
+      </c>
+      <c r="AA283">
+        <v>0</v>
+      </c>
+      <c r="AB283">
+        <v>0</v>
+      </c>
+      <c r="AC283">
+        <v>0</v>
+      </c>
+      <c r="AD283">
+        <v>0</v>
+      </c>
+      <c r="AE283">
+        <v>1</v>
+      </c>
+      <c r="AF283">
+        <v>0</v>
+      </c>
+      <c r="AG283">
+        <v>1</v>
+      </c>
+      <c r="AH283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A284">
+        <v>2024</v>
+      </c>
+      <c r="B284" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C284">
+        <v>42</v>
+      </c>
+      <c r="D284" t="s">
+        <v>46</v>
+      </c>
+      <c r="F284" t="s">
+        <v>13</v>
+      </c>
+      <c r="G284">
+        <v>6</v>
+      </c>
+      <c r="H284">
+        <v>2</v>
+      </c>
+      <c r="I284">
+        <v>3</v>
+      </c>
+      <c r="J284" t="s">
+        <v>37</v>
+      </c>
+      <c r="K284" t="s">
+        <v>31</v>
+      </c>
+      <c r="L284">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="M284">
+        <v>5</v>
+      </c>
+      <c r="N284">
+        <v>5</v>
+      </c>
+      <c r="O284">
+        <v>4</v>
+      </c>
+      <c r="P284">
+        <v>3</v>
+      </c>
+      <c r="Q284">
+        <v>6</v>
+      </c>
+      <c r="R284">
+        <v>4</v>
+      </c>
+      <c r="S284">
+        <v>5</v>
+      </c>
+      <c r="T284">
+        <v>4</v>
+      </c>
+      <c r="U284">
+        <v>5</v>
+      </c>
+      <c r="V284">
+        <v>2</v>
+      </c>
+      <c r="W284">
+        <v>0</v>
+      </c>
+      <c r="X284">
+        <v>0</v>
+      </c>
+      <c r="Y284">
+        <v>0</v>
+      </c>
+      <c r="Z284">
+        <v>0</v>
+      </c>
+      <c r="AA284">
+        <v>0</v>
+      </c>
+      <c r="AB284">
+        <v>0</v>
+      </c>
+      <c r="AC284">
+        <v>0</v>
+      </c>
+      <c r="AD284">
+        <v>0</v>
+      </c>
+      <c r="AE284">
+        <v>0</v>
+      </c>
+      <c r="AF284">
+        <v>0</v>
+      </c>
+      <c r="AG284">
+        <v>0</v>
+      </c>
+      <c r="AH284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A285">
+        <v>2024</v>
+      </c>
+      <c r="B285" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C285">
+        <v>43</v>
+      </c>
+      <c r="D285" t="s">
+        <v>46</v>
+      </c>
+      <c r="F285" t="s">
+        <v>12</v>
+      </c>
+      <c r="G285">
+        <v>8</v>
+      </c>
+      <c r="H285">
+        <v>2</v>
+      </c>
+      <c r="I285">
+        <v>2</v>
+      </c>
+      <c r="J285" t="s">
+        <v>36</v>
+      </c>
+      <c r="K285" t="s">
+        <v>31</v>
+      </c>
+      <c r="L285">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="M285">
+        <v>5</v>
+      </c>
+      <c r="N285">
+        <v>3</v>
+      </c>
+      <c r="O285">
+        <v>0</v>
+      </c>
+      <c r="P285">
+        <v>27</v>
+      </c>
+      <c r="Q285">
+        <v>5</v>
+      </c>
+      <c r="R285">
+        <v>4</v>
+      </c>
+      <c r="S285">
+        <v>0</v>
+      </c>
+      <c r="T285">
+        <v>0</v>
+      </c>
+      <c r="U285">
+        <v>0</v>
+      </c>
+      <c r="V285">
+        <v>0</v>
+      </c>
+      <c r="W285">
+        <v>0</v>
+      </c>
+      <c r="X285">
+        <v>0</v>
+      </c>
+      <c r="Y285">
+        <v>0</v>
+      </c>
+      <c r="Z285">
+        <v>0</v>
+      </c>
+      <c r="AA285">
+        <v>0</v>
+      </c>
+      <c r="AB285">
+        <v>0</v>
+      </c>
+      <c r="AC285">
+        <v>0</v>
+      </c>
+      <c r="AD285">
+        <v>0</v>
+      </c>
+      <c r="AE285">
+        <v>0</v>
+      </c>
+      <c r="AF285">
+        <v>1</v>
+      </c>
+      <c r="AG285">
+        <v>0</v>
+      </c>
+      <c r="AH285">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="286" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A286">
+        <v>2024</v>
+      </c>
+      <c r="B286" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C286">
+        <v>43</v>
+      </c>
+      <c r="D286" t="s">
+        <v>46</v>
+      </c>
+      <c r="F286" t="s">
+        <v>11</v>
+      </c>
+      <c r="G286">
+        <v>13</v>
+      </c>
+      <c r="H286">
+        <v>8</v>
+      </c>
+      <c r="I286">
+        <v>1</v>
+      </c>
+      <c r="J286" t="s">
+        <v>32</v>
+      </c>
+      <c r="K286" t="s">
+        <v>31</v>
+      </c>
+      <c r="L286">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="M286">
+        <v>6</v>
+      </c>
+      <c r="N286">
+        <v>4</v>
+      </c>
+      <c r="O286">
+        <v>5</v>
+      </c>
+      <c r="P286">
+        <v>0</v>
+      </c>
+      <c r="Q286">
+        <v>5</v>
+      </c>
+      <c r="R286">
+        <v>3</v>
+      </c>
+      <c r="S286">
+        <v>8</v>
+      </c>
+      <c r="T286">
+        <v>5</v>
+      </c>
+      <c r="U286">
+        <v>5</v>
+      </c>
+      <c r="V286">
+        <v>0</v>
+      </c>
+      <c r="W286">
+        <v>0</v>
+      </c>
+      <c r="X286">
+        <v>0</v>
+      </c>
+      <c r="Y286">
+        <v>0</v>
+      </c>
+      <c r="Z286">
+        <v>0</v>
+      </c>
+      <c r="AA286">
+        <v>0</v>
+      </c>
+      <c r="AB286">
+        <v>0</v>
+      </c>
+      <c r="AC286">
+        <v>1</v>
+      </c>
+      <c r="AD286">
+        <v>0</v>
+      </c>
+      <c r="AE286">
+        <v>1</v>
+      </c>
+      <c r="AF286">
+        <v>0</v>
+      </c>
+      <c r="AG286">
+        <v>0</v>
+      </c>
+      <c r="AH286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A287">
+        <v>2024</v>
+      </c>
+      <c r="B287" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C287">
+        <v>43</v>
+      </c>
+      <c r="D287" t="s">
+        <v>46</v>
+      </c>
+      <c r="F287" t="s">
+        <v>13</v>
+      </c>
+      <c r="G287">
+        <v>8</v>
+      </c>
+      <c r="H287">
+        <v>1</v>
+      </c>
+      <c r="I287">
+        <v>3</v>
+      </c>
+      <c r="J287" t="s">
+        <v>37</v>
+      </c>
+      <c r="K287" t="s">
+        <v>31</v>
+      </c>
+      <c r="L287">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="M287">
+        <v>5</v>
+      </c>
+      <c r="N287">
+        <v>5</v>
+      </c>
+      <c r="O287">
+        <v>7</v>
+      </c>
+      <c r="P287">
+        <v>8</v>
+      </c>
+      <c r="Q287">
+        <v>4</v>
+      </c>
+      <c r="R287">
+        <v>4</v>
+      </c>
+      <c r="S287">
+        <v>3</v>
+      </c>
+      <c r="T287">
+        <v>0</v>
+      </c>
+      <c r="U287">
+        <v>3</v>
+      </c>
+      <c r="V287">
+        <v>4</v>
+      </c>
+      <c r="W287">
+        <v>0</v>
+      </c>
+      <c r="X287">
+        <v>0</v>
+      </c>
+      <c r="Y287">
+        <v>0</v>
+      </c>
+      <c r="Z287">
+        <v>0</v>
+      </c>
+      <c r="AA287">
+        <v>0</v>
+      </c>
+      <c r="AB287">
+        <v>0</v>
+      </c>
+      <c r="AC287">
+        <v>0</v>
+      </c>
+      <c r="AD287">
+        <v>0</v>
+      </c>
+      <c r="AE287">
+        <v>0</v>
+      </c>
+      <c r="AF287">
+        <v>0</v>
+      </c>
+      <c r="AG287">
+        <v>0</v>
+      </c>
+      <c r="AH287">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="288" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A288">
+        <v>2024</v>
+      </c>
+      <c r="B288" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C288">
+        <v>44</v>
+      </c>
+      <c r="D288" t="s">
+        <v>46</v>
+      </c>
+      <c r="F288" t="s">
+        <v>12</v>
+      </c>
+      <c r="G288">
+        <v>8</v>
+      </c>
+      <c r="H288">
+        <v>2</v>
+      </c>
+      <c r="I288">
+        <v>2</v>
+      </c>
+      <c r="J288" t="s">
+        <v>36</v>
+      </c>
+      <c r="K288" t="s">
+        <v>31</v>
+      </c>
+      <c r="L288">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="M288">
+        <v>5</v>
+      </c>
+      <c r="N288">
+        <v>4</v>
+      </c>
+      <c r="O288">
+        <v>4</v>
+      </c>
+      <c r="P288">
+        <v>13</v>
+      </c>
+      <c r="Q288">
+        <v>4</v>
+      </c>
+      <c r="R288">
+        <v>10</v>
+      </c>
+      <c r="S288">
+        <v>0</v>
+      </c>
+      <c r="T288">
+        <v>0</v>
+      </c>
+      <c r="U288">
+        <v>0</v>
+      </c>
+      <c r="V288">
+        <v>0</v>
+      </c>
+      <c r="W288">
+        <v>0</v>
+      </c>
+      <c r="X288">
+        <v>0</v>
+      </c>
+      <c r="Y288">
+        <v>0</v>
+      </c>
+      <c r="Z288">
+        <v>0</v>
+      </c>
+      <c r="AA288">
+        <v>0</v>
+      </c>
+      <c r="AB288">
+        <v>0</v>
+      </c>
+      <c r="AC288">
+        <v>0</v>
+      </c>
+      <c r="AD288">
+        <v>0</v>
+      </c>
+      <c r="AE288">
+        <v>0</v>
+      </c>
+      <c r="AF288">
+        <v>1</v>
+      </c>
+      <c r="AG288">
+        <v>0</v>
+      </c>
+      <c r="AH288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A289">
+        <v>2024</v>
+      </c>
+      <c r="B289" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C289">
+        <v>44</v>
+      </c>
+      <c r="D289" t="s">
+        <v>46</v>
+      </c>
+      <c r="F289" t="s">
+        <v>13</v>
+      </c>
+      <c r="G289">
+        <v>5</v>
+      </c>
+      <c r="H289">
+        <v>1</v>
+      </c>
+      <c r="I289">
+        <v>3</v>
+      </c>
+      <c r="J289" t="s">
+        <v>32</v>
+      </c>
+      <c r="K289" t="s">
+        <v>31</v>
+      </c>
+      <c r="L289">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="M289">
+        <v>6</v>
+      </c>
+      <c r="N289">
+        <v>5</v>
+      </c>
+      <c r="O289">
+        <v>2</v>
+      </c>
+      <c r="P289">
+        <v>6</v>
+      </c>
+      <c r="Q289">
+        <v>5</v>
+      </c>
+      <c r="R289">
+        <v>3</v>
+      </c>
+      <c r="S289">
+        <v>8</v>
+      </c>
+      <c r="T289">
+        <v>2</v>
+      </c>
+      <c r="U289">
+        <v>0</v>
+      </c>
+      <c r="V289">
+        <v>5</v>
+      </c>
+      <c r="W289">
+        <v>0</v>
+      </c>
+      <c r="X289">
+        <v>0</v>
+      </c>
+      <c r="Y289">
+        <v>0</v>
+      </c>
+      <c r="Z289">
+        <v>0</v>
+      </c>
+      <c r="AA289">
+        <v>0</v>
+      </c>
+      <c r="AB289">
+        <v>0</v>
+      </c>
+      <c r="AC289">
+        <v>0</v>
+      </c>
+      <c r="AD289">
+        <v>0</v>
+      </c>
+      <c r="AE289">
+        <v>0</v>
+      </c>
+      <c r="AF289">
+        <v>0</v>
+      </c>
+      <c r="AG289">
+        <v>0</v>
+      </c>
+      <c r="AH289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A290">
+        <v>2024</v>
+      </c>
+      <c r="B290" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C290">
+        <v>44</v>
+      </c>
+      <c r="D290" t="s">
+        <v>46</v>
+      </c>
+      <c r="F290" t="s">
+        <v>11</v>
+      </c>
+      <c r="G290">
+        <v>13</v>
+      </c>
+      <c r="H290">
+        <v>5</v>
+      </c>
+      <c r="I290">
+        <v>1</v>
+      </c>
+      <c r="J290" t="s">
+        <v>37</v>
+      </c>
+      <c r="K290" t="s">
+        <v>31</v>
+      </c>
+      <c r="L290">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="M290">
+        <v>4</v>
+      </c>
+      <c r="N290">
+        <v>4</v>
+      </c>
+      <c r="O290">
+        <v>9</v>
+      </c>
+      <c r="P290">
+        <v>3</v>
+      </c>
+      <c r="Q290">
+        <v>0</v>
+      </c>
+      <c r="R290">
+        <v>2</v>
+      </c>
+      <c r="S290">
+        <v>9</v>
+      </c>
+      <c r="T290">
+        <v>9</v>
+      </c>
+      <c r="U290">
+        <v>0</v>
+      </c>
+      <c r="V290">
+        <v>0</v>
+      </c>
+      <c r="W290">
+        <v>0</v>
+      </c>
+      <c r="X290">
+        <v>0</v>
+      </c>
+      <c r="Y290">
+        <v>0</v>
+      </c>
+      <c r="Z290">
+        <v>0</v>
+      </c>
+      <c r="AA290">
+        <v>0</v>
+      </c>
+      <c r="AB290">
+        <v>0</v>
+      </c>
+      <c r="AC290">
+        <v>0</v>
+      </c>
+      <c r="AD290">
+        <v>1</v>
+      </c>
+      <c r="AE290">
+        <v>0</v>
+      </c>
+      <c r="AF290">
+        <v>0</v>
+      </c>
+      <c r="AG290">
+        <v>0</v>
+      </c>
+      <c r="AH290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A291">
+        <v>2024</v>
+      </c>
+      <c r="B291" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C291">
+        <v>45</v>
+      </c>
+      <c r="D291" t="s">
+        <v>46</v>
+      </c>
+      <c r="F291" t="s">
+        <v>12</v>
+      </c>
+      <c r="G291">
+        <v>13</v>
+      </c>
+      <c r="H291">
+        <v>5</v>
+      </c>
+      <c r="I291">
+        <v>1</v>
+      </c>
+      <c r="J291" t="s">
+        <v>36</v>
+      </c>
+      <c r="K291" t="s">
+        <v>31</v>
+      </c>
+      <c r="L291">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="M291">
+        <v>5</v>
+      </c>
+      <c r="N291">
+        <v>5</v>
+      </c>
+      <c r="O291">
+        <v>4</v>
+      </c>
+      <c r="P291">
+        <v>8</v>
+      </c>
+      <c r="Q291">
+        <v>3</v>
+      </c>
+      <c r="R291">
+        <v>5</v>
+      </c>
+      <c r="S291">
+        <v>4</v>
+      </c>
+      <c r="T291">
+        <v>0</v>
+      </c>
+      <c r="U291">
+        <v>1</v>
+      </c>
+      <c r="V291">
+        <v>3</v>
+      </c>
+      <c r="W291">
+        <v>0</v>
+      </c>
+      <c r="X291">
+        <v>0</v>
+      </c>
+      <c r="Y291">
+        <v>0</v>
+      </c>
+      <c r="Z291">
+        <v>0</v>
+      </c>
+      <c r="AA291">
+        <v>0</v>
+      </c>
+      <c r="AB291">
+        <v>0</v>
+      </c>
+      <c r="AC291">
+        <v>0</v>
+      </c>
+      <c r="AD291">
+        <v>0</v>
+      </c>
+      <c r="AE291">
+        <v>0</v>
+      </c>
+      <c r="AF291">
+        <v>0</v>
+      </c>
+      <c r="AG291">
+        <v>0</v>
+      </c>
+      <c r="AH291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A292">
+        <v>2024</v>
+      </c>
+      <c r="B292" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C292">
+        <v>45</v>
+      </c>
+      <c r="D292" t="s">
+        <v>46</v>
+      </c>
+      <c r="F292" t="s">
+        <v>13</v>
+      </c>
+      <c r="G292">
+        <v>10</v>
+      </c>
+      <c r="H292">
+        <v>2</v>
+      </c>
+      <c r="I292">
+        <v>2</v>
+      </c>
+      <c r="J292" t="s">
+        <v>32</v>
+      </c>
+      <c r="K292" t="s">
+        <v>31</v>
+      </c>
+      <c r="L292">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="M292">
+        <v>5</v>
+      </c>
+      <c r="N292">
+        <v>5</v>
+      </c>
+      <c r="O292">
+        <v>2</v>
+      </c>
+      <c r="P292">
+        <v>5</v>
+      </c>
+      <c r="Q292">
+        <v>3</v>
+      </c>
+      <c r="R292">
+        <v>12</v>
+      </c>
+      <c r="S292">
+        <v>3</v>
+      </c>
+      <c r="T292">
+        <v>2</v>
+      </c>
+      <c r="U292">
+        <v>0</v>
+      </c>
+      <c r="V292">
+        <v>3</v>
+      </c>
+      <c r="W292">
+        <v>0</v>
+      </c>
+      <c r="X292">
+        <v>0</v>
+      </c>
+      <c r="Y292">
+        <v>0</v>
+      </c>
+      <c r="Z292">
+        <v>0</v>
+      </c>
+      <c r="AA292">
+        <v>0</v>
+      </c>
+      <c r="AB292">
+        <v>0</v>
+      </c>
+      <c r="AC292">
+        <v>0</v>
+      </c>
+      <c r="AD292">
+        <v>0</v>
+      </c>
+      <c r="AE292">
+        <v>0</v>
+      </c>
+      <c r="AF292">
+        <v>0</v>
+      </c>
+      <c r="AG292">
+        <v>0</v>
+      </c>
+      <c r="AH292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:34" x14ac:dyDescent="0.35">
+      <c r="A293">
+        <v>2024</v>
+      </c>
+      <c r="B293" s="5">
+        <v>45646</v>
+      </c>
+      <c r="C293">
+        <v>45</v>
+      </c>
+      <c r="D293" t="s">
+        <v>46</v>
+      </c>
+      <c r="F293" t="s">
+        <v>11</v>
+      </c>
+      <c r="G293">
+        <v>9</v>
+      </c>
+      <c r="H293">
+        <v>2</v>
+      </c>
+      <c r="I293">
+        <v>3</v>
+      </c>
+      <c r="J293" t="s">
+        <v>37</v>
+      </c>
+      <c r="K293" t="s">
+        <v>31</v>
+      </c>
+      <c r="L293">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="M293">
+        <v>5</v>
+      </c>
+      <c r="N293">
+        <v>5</v>
+      </c>
+      <c r="O293">
+        <v>5</v>
+      </c>
+      <c r="P293">
+        <v>3</v>
+      </c>
+      <c r="Q293">
+        <v>6</v>
+      </c>
+      <c r="R293">
+        <v>5</v>
+      </c>
+      <c r="S293">
+        <v>2</v>
+      </c>
+      <c r="T293">
+        <v>5</v>
+      </c>
+      <c r="U293">
+        <v>2</v>
+      </c>
+      <c r="V293">
+        <v>3</v>
+      </c>
+      <c r="W293">
+        <v>0</v>
+      </c>
+      <c r="X293">
+        <v>0</v>
+      </c>
+      <c r="Y293">
+        <v>0</v>
+      </c>
+      <c r="Z293">
+        <v>0</v>
+      </c>
+      <c r="AA293">
+        <v>0</v>
+      </c>
+      <c r="AB293">
+        <v>0</v>
+      </c>
+      <c r="AC293">
+        <v>0</v>
+      </c>
+      <c r="AD293">
+        <v>1</v>
+      </c>
+      <c r="AE293">
+        <v>0</v>
+      </c>
+      <c r="AF293">
+        <v>0</v>
+      </c>
+      <c r="AG293">
+        <v>0</v>
+      </c>
+      <c r="AH293">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:AP272" xr:uid="{FF8635BA-0A9D-4832-9FDC-B5CDD32D9D6C}"/>
+  <autoFilter ref="A2:AP290" xr:uid="{FF8635BA-0A9D-4832-9FDC-B5CDD32D9D6C}"/>
   <dataValidations count="1">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:AB8 W3:X41 Y9:Z41 W44:Z56 X58:Z116 X117:AB119 X120:Z122 X123:AB128 W58:W175 X129:Z175 W177:Z223 W225:Z1048576" xr:uid="{0D054DE4-3D8E-4484-9FF1-661236EA2207}">
       <formula1>0</formula1>

</xml_diff>